<commit_message>
'Share_This_Bot' to 'Share_This_App' (#30)
* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_A5315D46_C6C3_49F2_A561_52C920B09F45_.wvu.FilterData">'client strings'!$F$1:$F$1384</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_B2B3A515_AAAE_4B85_AA8F_07109D850492_.wvu.FilterData">'client strings'!$C$1:$C$1384</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_26672240_873B_4542_BA47_A8A4A43A62A3_.wvu.FilterData">'client strings'!$F$1:$F$1384</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_3A0E1F6B_18F2_40C0_B26B_84887283C8F8_.wvu.FilterData">'client strings'!$C$1:$C$1384</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B2B3A515-AAAE-4B85-AA8F-07109D850492}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A5315D46-C6C3-49F2-A561-52C920B09F45}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3A0E1F6B-18F2-40C0-B26B-84887283C8F8}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{26672240-873B-4542-BA47-A8A4A43A62A3}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13407" uniqueCount="6190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13407" uniqueCount="6188">
   <si>
     <t>platform</t>
   </si>
@@ -11741,7 +11741,7 @@
     <t>photo.count</t>
   </si>
   <si>
-    <t>%1$d  Photos</t>
+    <t>%1$d Photos</t>
   </si>
   <si>
     <t>%1$d 张图片</t>
@@ -14996,16 +14996,16 @@
     <t>QRコードを共有</t>
   </si>
   <si>
-    <t>Share_This_Bot</t>
-  </si>
-  <si>
-    <t>Share This Bot</t>
+    <t>Share_This_App</t>
+  </si>
+  <si>
+    <t>Share This App</t>
   </si>
   <si>
     <t>Kongsi Aplikasi Ini</t>
   </si>
   <si>
-    <t>分享机器人</t>
+    <t>分享应用</t>
   </si>
   <si>
     <t>このアプリをシェアする</t>
@@ -18332,7 +18332,7 @@
     <t>最初のリストを作成して、\n自分の好きなユーザーやミニアプリを追加しましょう</t>
   </si>
   <si>
-    <t>%1$dの会話</t>
+    <t>w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w w</t>
   </si>
   <si>
     <t>%1$d個</t>
@@ -18621,12 +18621,6 @@
   </si>
   <si>
     <t>Are you sure you want to send the %1$s ?</t>
-  </si>
-  <si>
-    <t>Share_This_App</t>
-  </si>
-  <si>
-    <t>Share This App</t>
   </si>
   <si>
     <t>The current version (%1$s) is no longer avaliable!\nPlease click "Update" below to update to the latest version from the Google Play.</t>
@@ -48116,10 +48110,10 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{A5315D46-C6C3-49F2-A561-52C920B09F45}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{26672240-873B-4542-BA47-A8A4A43A62A3}" filter="1" showAutoFilter="1">
       <autoFilter ref="$F$1:$F$1384"/>
     </customSheetView>
-    <customSheetView guid="{B2B3A515-AAAE-4B85-AA8F-07109D850492}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{3A0E1F6B-18F2-40C0-B26B-84887283C8F8}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1384"/>
     </customSheetView>
   </customSheetViews>
@@ -63117,10 +63111,10 @@
         <v>72</v>
       </c>
       <c r="B1076" s="20" t="s">
-        <v>6180</v>
+        <v>4971</v>
       </c>
       <c r="C1076" s="20" t="s">
-        <v>6181</v>
+        <v>4972</v>
       </c>
       <c r="D1076" s="49" t="s">
         <v>4975</v>
@@ -64874,7 +64868,7 @@
         <v>5529</v>
       </c>
       <c r="C1205" s="20" t="s">
-        <v>6182</v>
+        <v>6180</v>
       </c>
       <c r="D1205" s="49"/>
     </row>
@@ -65094,7 +65088,7 @@
         <v>5600</v>
       </c>
       <c r="C1221" s="20" t="s">
-        <v>6183</v>
+        <v>6181</v>
       </c>
       <c r="D1221" s="49" t="s">
         <v>5603</v>
@@ -65891,7 +65885,7 @@
         <v>5464</v>
       </c>
       <c r="D1278" s="50" t="s">
-        <v>6184</v>
+        <v>6182</v>
       </c>
     </row>
     <row r="1279">
@@ -65905,7 +65899,7 @@
         <v>5872</v>
       </c>
       <c r="D1279" s="50" t="s">
-        <v>6185</v>
+        <v>6183</v>
       </c>
     </row>
     <row r="1280">
@@ -66295,7 +66289,7 @@
         <v>6009</v>
       </c>
       <c r="D1307" s="55" t="s">
-        <v>6186</v>
+        <v>6184</v>
       </c>
     </row>
     <row r="1308">
@@ -66669,7 +66663,7 @@
         <v>124</v>
       </c>
       <c r="B1337" s="20" t="s">
-        <v>6187</v>
+        <v>6185</v>
       </c>
       <c r="C1337" s="27" t="s">
         <v>6158</v>
@@ -66723,7 +66717,7 @@
         <v>4278</v>
       </c>
       <c r="D1341" s="55" t="s">
-        <v>6188</v>
+        <v>6186</v>
       </c>
     </row>
     <row r="1342">
@@ -66923,7 +66917,7 @@
         <v>5893</v>
       </c>
       <c r="D1357" s="55" t="s">
-        <v>6189</v>
+        <v>6187</v>
       </c>
     </row>
     <row r="1358">

</xml_diff>

<commit_message>
Add lowercase 'you' (#34)
* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_B7574AD3_380E_4596_B289_B818D6FBD61C_.wvu.FilterData">'client strings'!$C$1:$C$1388</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D85AB609_9F50_4029_B867_2BD7C2E3B1F3_.wvu.FilterData">'client strings'!$F$1:$F$1388</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_7239FA5E_7AC2_4C1E_AE5A_E61676447D4F_.wvu.FilterData">'client strings'!$F$1:$F$1389</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D0E86AF8_F90D_4519_9F1B_CEE6A21F9473_.wvu.FilterData">'client strings'!$C$1:$C$1389</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B7574AD3-380E-4596-B289-B818D6FBD61C}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D85AB609-9F50-4029-B867-2BD7C2E3B1F3}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D0E86AF8-F90D-4519-9F1B-CEE6A21F9473}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7239FA5E-7AC2-4C1E-AE5A-E61676447D4F}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13548" uniqueCount="6332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13552" uniqueCount="6333">
   <si>
     <t>platform</t>
   </si>
@@ -18179,13 +18179,16 @@
     <t>Tulis Lingkaran</t>
   </si>
   <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>你</t>
+  </si>
+  <si>
     <t>You</t>
   </si>
   <si>
     <t>Anda</t>
-  </si>
-  <si>
-    <t>你</t>
   </si>
   <si>
     <t>自分</t>
@@ -48455,105 +48458,103 @@
     </row>
     <row r="1381" ht="15.75" customHeight="1">
       <c r="A1381" s="1" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B1381" s="1" t="s">
         <v>6032</v>
       </c>
-      <c r="C1381" s="4" t="s">
+      <c r="C1381" s="1" t="s">
         <v>6032</v>
       </c>
-      <c r="D1381" s="4" t="s">
+      <c r="D1381" s="4"/>
+      <c r="E1381" s="4"/>
+      <c r="F1381" s="1" t="s">
         <v>6033</v>
       </c>
-      <c r="E1381" s="4" t="s">
-        <v>6033</v>
-      </c>
-      <c r="F1381" s="4" t="s">
-        <v>6034</v>
-      </c>
-      <c r="G1381" s="3" t="s">
-        <v>6035</v>
-      </c>
+      <c r="G1381" s="3"/>
     </row>
     <row r="1382" ht="15.75" customHeight="1">
       <c r="A1382" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1382" s="1" t="s">
+        <v>6034</v>
+      </c>
+      <c r="C1382" s="4" t="s">
+        <v>6034</v>
+      </c>
+      <c r="D1382" s="4" t="s">
+        <v>6035</v>
+      </c>
+      <c r="E1382" s="4" t="s">
+        <v>6035</v>
+      </c>
+      <c r="F1382" s="4" t="s">
+        <v>6033</v>
+      </c>
+      <c r="G1382" s="3" t="s">
         <v>6036</v>
-      </c>
-      <c r="C1382" s="4" t="s">
-        <v>6037</v>
-      </c>
-      <c r="D1382" s="4" t="s">
-        <v>6038</v>
-      </c>
-      <c r="E1382" s="4" t="s">
-        <v>6039</v>
-      </c>
-      <c r="F1382" s="4" t="s">
-        <v>6040</v>
-      </c>
-      <c r="G1382" s="3" t="s">
-        <v>6041</v>
       </c>
     </row>
     <row r="1383" ht="15.75" customHeight="1">
       <c r="A1383" s="1" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="B1383" s="1" t="s">
+        <v>6037</v>
+      </c>
+      <c r="C1383" s="4" t="s">
+        <v>6038</v>
+      </c>
+      <c r="D1383" s="4" t="s">
+        <v>6039</v>
+      </c>
+      <c r="E1383" s="4" t="s">
+        <v>6040</v>
+      </c>
+      <c r="F1383" s="4" t="s">
+        <v>6041</v>
+      </c>
+      <c r="G1383" s="3" t="s">
         <v>6042</v>
-      </c>
-      <c r="C1383" s="1" t="s">
-        <v>6043</v>
-      </c>
-      <c r="D1383" s="4"/>
-      <c r="E1383" s="4"/>
-      <c r="F1383" s="1" t="s">
-        <v>6044</v>
-      </c>
-      <c r="G1383" s="7" t="s">
-        <v>6045</v>
       </c>
     </row>
     <row r="1384" ht="15.75" customHeight="1">
       <c r="A1384" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B1384" s="1" t="s">
-        <v>6046</v>
+        <v>6043</v>
       </c>
       <c r="C1384" s="1" t="s">
-        <v>6047</v>
+        <v>6044</v>
       </c>
       <c r="D1384" s="4"/>
       <c r="E1384" s="4"/>
-      <c r="F1384" s="4" t="s">
-        <v>6048</v>
-      </c>
-      <c r="G1384" s="3" t="s">
-        <v>6049</v>
+      <c r="F1384" s="1" t="s">
+        <v>6045</v>
+      </c>
+      <c r="G1384" s="7" t="s">
+        <v>6046</v>
       </c>
     </row>
     <row r="1385" ht="15.75" customHeight="1">
       <c r="A1385" s="1" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="B1385" s="1" t="s">
-        <v>6050</v>
+        <v>6047</v>
       </c>
       <c r="C1385" s="1" t="s">
-        <v>6051</v>
+        <v>6048</v>
       </c>
       <c r="D1385" s="4"/>
       <c r="E1385" s="4"/>
-      <c r="F1385" s="1" t="s">
-        <v>891</v>
-      </c>
-      <c r="G1385" s="7" t="s">
-        <v>6052</v>
+      <c r="F1385" s="4" t="s">
+        <v>6049</v>
+      </c>
+      <c r="G1385" s="3" t="s">
+        <v>6050</v>
       </c>
     </row>
     <row r="1386" ht="15.75" customHeight="1">
@@ -48561,18 +48562,18 @@
         <v>105</v>
       </c>
       <c r="B1386" s="1" t="s">
-        <v>6053</v>
+        <v>6051</v>
       </c>
       <c r="C1386" s="1" t="s">
-        <v>6054</v>
+        <v>6052</v>
       </c>
       <c r="D1386" s="4"/>
       <c r="E1386" s="4"/>
       <c r="F1386" s="1" t="s">
-        <v>6055</v>
+        <v>891</v>
       </c>
       <c r="G1386" s="7" t="s">
-        <v>6056</v>
+        <v>6053</v>
       </c>
     </row>
     <row r="1387" ht="15.75" customHeight="1">
@@ -48580,59 +48581,78 @@
         <v>105</v>
       </c>
       <c r="B1387" s="1" t="s">
-        <v>6057</v>
+        <v>6054</v>
       </c>
       <c r="C1387" s="1" t="s">
-        <v>6058</v>
+        <v>6055</v>
       </c>
       <c r="D1387" s="4"/>
       <c r="E1387" s="4"/>
       <c r="F1387" s="1" t="s">
-        <v>912</v>
+        <v>6056</v>
       </c>
       <c r="G1387" s="7" t="s">
-        <v>6059</v>
+        <v>6057</v>
       </c>
     </row>
     <row r="1388" ht="15.75" customHeight="1">
       <c r="A1388" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B1388" s="1" t="s">
-        <v>6060</v>
+        <v>6058</v>
       </c>
       <c r="C1388" s="1" t="s">
-        <v>6061</v>
+        <v>6059</v>
       </c>
       <c r="D1388" s="4"/>
       <c r="E1388" s="4"/>
       <c r="F1388" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="G1388" s="7" t="s">
+        <v>6060</v>
+      </c>
+    </row>
+    <row r="1389" ht="15.75" customHeight="1">
+      <c r="A1389" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1389" s="1" t="s">
+        <v>6061</v>
+      </c>
+      <c r="C1389" s="1" t="s">
         <v>6062</v>
       </c>
-      <c r="G1388" s="7"/>
+      <c r="D1389" s="4"/>
+      <c r="E1389" s="4"/>
+      <c r="F1389" s="1" t="s">
+        <v>6063</v>
+      </c>
+      <c r="G1389" s="7"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D85AB609-9F50-4029-B867-2BD7C2E3B1F3}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$F$1:$F$1388"/>
+    <customSheetView guid="{7239FA5E-7AC2-4C1E-AE5A-E61676447D4F}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$F$1:$F$1389"/>
     </customSheetView>
-    <customSheetView guid="{B7574AD3-380E-4596-B289-B818D6FBD61C}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$C$1:$C$1388"/>
+    <customSheetView guid="{D0E86AF8-F90D-4519-9F1B-CEE6A21F9473}" filter="1" showAutoFilter="1">
+      <autoFilter ref="$C$1:$C$1389"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="B159:B160">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF(C159:C1506, B159) &gt; 1</formula>
+      <formula>COUNTIF(C159:C1507, B159) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B146">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>COUNTIF(C121:C1485, B121) &gt; 1</formula>
+      <formula>COUNTIF(C121:C1486, B121) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B148:B158">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COUNTIF(C148:C1486, B148) &gt; 1</formula>
+      <formula>COUNTIF(C148:C1487, B148) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -48898,10 +48918,10 @@
         <v>72</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>6063</v>
+        <v>6064</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>6064</v>
+        <v>6065</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>78</v>
@@ -49800,7 +49820,7 @@
         <v>263</v>
       </c>
       <c r="D81" s="49" t="s">
-        <v>6065</v>
+        <v>6066</v>
       </c>
     </row>
     <row r="82">
@@ -50004,10 +50024,10 @@
         <v>105</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>6066</v>
+        <v>6067</v>
       </c>
       <c r="C96" s="52" t="s">
-        <v>6067</v>
+        <v>6068</v>
       </c>
       <c r="D96" s="22" t="s">
         <v>731</v>
@@ -50024,7 +50044,7 @@
         <v>464</v>
       </c>
       <c r="D97" s="54" t="s">
-        <v>6068</v>
+        <v>6069</v>
       </c>
     </row>
     <row r="98">
@@ -50318,7 +50338,7 @@
         <v>584</v>
       </c>
       <c r="D118" s="49" t="s">
-        <v>6069</v>
+        <v>6070</v>
       </c>
     </row>
     <row r="119">
@@ -50486,7 +50506,7 @@
         <v>598</v>
       </c>
       <c r="D130" s="54" t="s">
-        <v>6070</v>
+        <v>6071</v>
       </c>
     </row>
     <row r="131">
@@ -50500,7 +50520,7 @@
         <v>604</v>
       </c>
       <c r="D131" s="54" t="s">
-        <v>6071</v>
+        <v>6072</v>
       </c>
     </row>
     <row r="132">
@@ -50598,7 +50618,7 @@
         <v>640</v>
       </c>
       <c r="D138" s="49" t="s">
-        <v>6072</v>
+        <v>6073</v>
       </c>
     </row>
     <row r="139">
@@ -50682,7 +50702,7 @@
         <v>670</v>
       </c>
       <c r="D144" s="57" t="s">
-        <v>6073</v>
+        <v>6074</v>
       </c>
     </row>
     <row r="145">
@@ -50752,7 +50772,7 @@
         <v>692</v>
       </c>
       <c r="D149" s="49" t="s">
-        <v>6074</v>
+        <v>6075</v>
       </c>
     </row>
     <row r="150">
@@ -50878,7 +50898,7 @@
         <v>741</v>
       </c>
       <c r="D158" s="48" t="s">
-        <v>6075</v>
+        <v>6076</v>
       </c>
     </row>
     <row r="159">
@@ -50920,7 +50940,7 @@
         <v>749</v>
       </c>
       <c r="D161" s="49" t="s">
-        <v>6076</v>
+        <v>6077</v>
       </c>
     </row>
     <row r="162">
@@ -51032,7 +51052,7 @@
         <v>782</v>
       </c>
       <c r="D169" s="58" t="s">
-        <v>6077</v>
+        <v>6078</v>
       </c>
     </row>
     <row r="170">
@@ -51088,7 +51108,7 @@
         <v>812</v>
       </c>
       <c r="D173" s="49" t="s">
-        <v>6078</v>
+        <v>6079</v>
       </c>
     </row>
     <row r="174">
@@ -51158,7 +51178,7 @@
         <v>835</v>
       </c>
       <c r="D178" s="49" t="s">
-        <v>6079</v>
+        <v>6080</v>
       </c>
     </row>
     <row r="179">
@@ -51494,7 +51514,7 @@
         <v>948</v>
       </c>
       <c r="D202" s="49" t="s">
-        <v>6080</v>
+        <v>6081</v>
       </c>
     </row>
     <row r="203">
@@ -51516,13 +51536,13 @@
         <v>53</v>
       </c>
       <c r="B204" s="22" t="s">
-        <v>6081</v>
+        <v>6082</v>
       </c>
       <c r="C204" s="22" t="s">
         <v>978</v>
       </c>
       <c r="D204" s="57" t="s">
-        <v>6082</v>
+        <v>6083</v>
       </c>
     </row>
     <row r="205">
@@ -51578,7 +51598,7 @@
         <v>975</v>
       </c>
       <c r="D208" s="49" t="s">
-        <v>6083</v>
+        <v>6084</v>
       </c>
     </row>
     <row r="209">
@@ -51631,7 +51651,7 @@
         <v>996</v>
       </c>
       <c r="C212" s="52" t="s">
-        <v>6084</v>
+        <v>6085</v>
       </c>
       <c r="D212" s="48" t="s">
         <v>999</v>
@@ -51648,7 +51668,7 @@
         <v>1001</v>
       </c>
       <c r="D213" s="49" t="s">
-        <v>6085</v>
+        <v>6086</v>
       </c>
     </row>
     <row r="214">
@@ -51662,7 +51682,7 @@
         <v>1003</v>
       </c>
       <c r="D214" s="49" t="s">
-        <v>6085</v>
+        <v>6086</v>
       </c>
     </row>
     <row r="215">
@@ -51872,7 +51892,7 @@
         <v>1082</v>
       </c>
       <c r="D229" s="58" t="s">
-        <v>6086</v>
+        <v>6087</v>
       </c>
     </row>
     <row r="230">
@@ -51900,7 +51920,7 @@
         <v>1093</v>
       </c>
       <c r="D231" s="49" t="s">
-        <v>6087</v>
+        <v>6088</v>
       </c>
     </row>
     <row r="232">
@@ -51914,7 +51934,7 @@
         <v>1088</v>
       </c>
       <c r="D232" s="49" t="s">
-        <v>6088</v>
+        <v>6089</v>
       </c>
     </row>
     <row r="233">
@@ -51925,10 +51945,10 @@
         <v>1095</v>
       </c>
       <c r="C233" s="52" t="s">
-        <v>6089</v>
+        <v>6090</v>
       </c>
       <c r="D233" s="48" t="s">
-        <v>6090</v>
+        <v>6091</v>
       </c>
     </row>
     <row r="234">
@@ -51956,7 +51976,7 @@
         <v>1105</v>
       </c>
       <c r="D235" s="49" t="s">
-        <v>6091</v>
+        <v>6092</v>
       </c>
     </row>
     <row r="236">
@@ -51998,7 +52018,7 @@
         <v>1118</v>
       </c>
       <c r="D238" s="49" t="s">
-        <v>6092</v>
+        <v>6093</v>
       </c>
     </row>
     <row r="239">
@@ -52124,7 +52144,7 @@
         <v>1162</v>
       </c>
       <c r="D247" s="49" t="s">
-        <v>6093</v>
+        <v>6094</v>
       </c>
     </row>
     <row r="248">
@@ -52152,7 +52172,7 @@
         <v>1174</v>
       </c>
       <c r="D249" s="49" t="s">
-        <v>6094</v>
+        <v>6095</v>
       </c>
     </row>
     <row r="250">
@@ -52194,7 +52214,7 @@
         <v>1184</v>
       </c>
       <c r="D252" s="57" t="s">
-        <v>6095</v>
+        <v>6096</v>
       </c>
     </row>
     <row r="253">
@@ -52208,7 +52228,7 @@
         <v>1187</v>
       </c>
       <c r="D253" s="57" t="s">
-        <v>6095</v>
+        <v>6096</v>
       </c>
     </row>
     <row r="254">
@@ -52222,7 +52242,7 @@
         <v>1191</v>
       </c>
       <c r="D254" s="49" t="s">
-        <v>6096</v>
+        <v>6097</v>
       </c>
     </row>
     <row r="255">
@@ -52236,7 +52256,7 @@
         <v>1194</v>
       </c>
       <c r="D255" s="49" t="s">
-        <v>6097</v>
+        <v>6098</v>
       </c>
     </row>
     <row r="256">
@@ -52362,7 +52382,7 @@
         <v>1234</v>
       </c>
       <c r="D264" s="49" t="s">
-        <v>6098</v>
+        <v>6099</v>
       </c>
     </row>
     <row r="265">
@@ -52614,7 +52634,7 @@
         <v>1305</v>
       </c>
       <c r="D282" s="57" t="s">
-        <v>6099</v>
+        <v>6100</v>
       </c>
     </row>
     <row r="283">
@@ -52628,7 +52648,7 @@
         <v>1308</v>
       </c>
       <c r="D283" s="57" t="s">
-        <v>6099</v>
+        <v>6100</v>
       </c>
     </row>
     <row r="284">
@@ -52642,7 +52662,7 @@
         <v>1312</v>
       </c>
       <c r="D284" s="49" t="s">
-        <v>6100</v>
+        <v>6101</v>
       </c>
     </row>
     <row r="285">
@@ -52667,7 +52687,7 @@
         <v>1322</v>
       </c>
       <c r="C286" s="22" t="s">
-        <v>6101</v>
+        <v>6102</v>
       </c>
       <c r="D286" s="48" t="s">
         <v>1327</v>
@@ -52748,10 +52768,10 @@
         <v>72</v>
       </c>
       <c r="B292" s="22" t="s">
-        <v>6102</v>
+        <v>6103</v>
       </c>
       <c r="C292" s="22" t="s">
-        <v>6103</v>
+        <v>6104</v>
       </c>
       <c r="D292" s="48" t="s">
         <v>1357</v>
@@ -53314,7 +53334,7 @@
         <v>1531</v>
       </c>
       <c r="D332" s="54" t="s">
-        <v>6104</v>
+        <v>6105</v>
       </c>
     </row>
     <row r="333">
@@ -53328,7 +53348,7 @@
         <v>1534</v>
       </c>
       <c r="D333" s="62" t="s">
-        <v>6105</v>
+        <v>6106</v>
       </c>
     </row>
     <row r="334">
@@ -53342,7 +53362,7 @@
         <v>1537</v>
       </c>
       <c r="D334" s="49" t="s">
-        <v>6106</v>
+        <v>6107</v>
       </c>
     </row>
     <row r="335">
@@ -53440,7 +53460,7 @@
         <v>1568</v>
       </c>
       <c r="D341" s="49" t="s">
-        <v>6107</v>
+        <v>6108</v>
       </c>
     </row>
     <row r="342">
@@ -53482,7 +53502,7 @@
         <v>1577</v>
       </c>
       <c r="D344" s="49" t="s">
-        <v>6108</v>
+        <v>6109</v>
       </c>
     </row>
     <row r="345">
@@ -53510,7 +53530,7 @@
         <v>1587</v>
       </c>
       <c r="D346" s="49" t="s">
-        <v>6109</v>
+        <v>6110</v>
       </c>
     </row>
     <row r="347">
@@ -53902,7 +53922,7 @@
         <v>1711</v>
       </c>
       <c r="D374" s="49" t="s">
-        <v>6110</v>
+        <v>6111</v>
       </c>
     </row>
     <row r="375">
@@ -53958,7 +53978,7 @@
         <v>1725</v>
       </c>
       <c r="D378" s="49" t="s">
-        <v>6111</v>
+        <v>6112</v>
       </c>
     </row>
     <row r="379">
@@ -54000,7 +54020,7 @@
         <v>1740</v>
       </c>
       <c r="D381" s="49" t="s">
-        <v>6112</v>
+        <v>6113</v>
       </c>
     </row>
     <row r="382">
@@ -54014,7 +54034,7 @@
         <v>1743</v>
       </c>
       <c r="D382" s="49" t="s">
-        <v>6112</v>
+        <v>6113</v>
       </c>
     </row>
     <row r="383">
@@ -54042,7 +54062,7 @@
         <v>1751</v>
       </c>
       <c r="D384" s="49" t="s">
-        <v>6113</v>
+        <v>6114</v>
       </c>
     </row>
     <row r="385">
@@ -54056,7 +54076,7 @@
         <v>1755</v>
       </c>
       <c r="D385" s="58" t="s">
-        <v>6114</v>
+        <v>6115</v>
       </c>
     </row>
     <row r="386">
@@ -54098,7 +54118,7 @@
         <v>1772</v>
       </c>
       <c r="D388" s="49" t="s">
-        <v>6115</v>
+        <v>6116</v>
       </c>
     </row>
     <row r="389">
@@ -54112,7 +54132,7 @@
         <v>1777</v>
       </c>
       <c r="D389" s="49" t="s">
-        <v>6116</v>
+        <v>6117</v>
       </c>
     </row>
     <row r="390">
@@ -54126,7 +54146,7 @@
         <v>1782</v>
       </c>
       <c r="D390" s="49" t="s">
-        <v>6117</v>
+        <v>6118</v>
       </c>
     </row>
     <row r="391">
@@ -54168,7 +54188,7 @@
         <v>1794</v>
       </c>
       <c r="D393" s="49" t="s">
-        <v>6118</v>
+        <v>6119</v>
       </c>
     </row>
     <row r="394">
@@ -54308,7 +54328,7 @@
         <v>1834</v>
       </c>
       <c r="D403" s="49" t="s">
-        <v>6119</v>
+        <v>6120</v>
       </c>
     </row>
     <row r="404">
@@ -54322,7 +54342,7 @@
         <v>1838</v>
       </c>
       <c r="D404" s="49" t="s">
-        <v>6120</v>
+        <v>6121</v>
       </c>
     </row>
     <row r="405">
@@ -54336,7 +54356,7 @@
         <v>1841</v>
       </c>
       <c r="D405" s="49" t="s">
-        <v>6121</v>
+        <v>6122</v>
       </c>
     </row>
     <row r="406">
@@ -54350,7 +54370,7 @@
         <v>1844</v>
       </c>
       <c r="D406" s="49" t="s">
-        <v>6122</v>
+        <v>6123</v>
       </c>
     </row>
     <row r="407">
@@ -54364,7 +54384,7 @@
         <v>1848</v>
       </c>
       <c r="D407" s="49" t="s">
-        <v>6123</v>
+        <v>6124</v>
       </c>
     </row>
     <row r="408">
@@ -54378,7 +54398,7 @@
         <v>1851</v>
       </c>
       <c r="D408" s="49" t="s">
-        <v>6124</v>
+        <v>6125</v>
       </c>
     </row>
     <row r="409">
@@ -54406,7 +54426,7 @@
         <v>1856</v>
       </c>
       <c r="D410" s="49" t="s">
-        <v>6125</v>
+        <v>6126</v>
       </c>
     </row>
     <row r="411">
@@ -54420,7 +54440,7 @@
         <v>1859</v>
       </c>
       <c r="D411" s="49" t="s">
-        <v>6126</v>
+        <v>6127</v>
       </c>
     </row>
     <row r="412">
@@ -54434,7 +54454,7 @@
         <v>1862</v>
       </c>
       <c r="D412" s="49" t="s">
-        <v>6127</v>
+        <v>6128</v>
       </c>
     </row>
     <row r="413">
@@ -54448,7 +54468,7 @@
         <v>1865</v>
       </c>
       <c r="D413" s="54" t="s">
-        <v>6128</v>
+        <v>6129</v>
       </c>
     </row>
     <row r="414">
@@ -54728,7 +54748,7 @@
         <v>1964</v>
       </c>
       <c r="D433" s="54" t="s">
-        <v>6129</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="434">
@@ -54826,7 +54846,7 @@
         <v>1989</v>
       </c>
       <c r="D440" s="54" t="s">
-        <v>6130</v>
+        <v>6131</v>
       </c>
     </row>
     <row r="441">
@@ -54924,7 +54944,7 @@
         <v>2019</v>
       </c>
       <c r="D447" s="54" t="s">
-        <v>6131</v>
+        <v>6132</v>
       </c>
     </row>
     <row r="448">
@@ -55302,7 +55322,7 @@
         <v>2153</v>
       </c>
       <c r="D474" s="54" t="s">
-        <v>6132</v>
+        <v>6133</v>
       </c>
     </row>
     <row r="475">
@@ -55484,7 +55504,7 @@
         <v>2231</v>
       </c>
       <c r="D487" s="54" t="s">
-        <v>6133</v>
+        <v>6134</v>
       </c>
     </row>
     <row r="488">
@@ -55498,7 +55518,7 @@
         <v>2234</v>
       </c>
       <c r="D488" s="54" t="s">
-        <v>6134</v>
+        <v>6135</v>
       </c>
     </row>
     <row r="489">
@@ -55554,7 +55574,7 @@
         <v>2253</v>
       </c>
       <c r="D492" s="54" t="s">
-        <v>6135</v>
+        <v>6136</v>
       </c>
     </row>
     <row r="493">
@@ -55638,7 +55658,7 @@
         <v>2284</v>
       </c>
       <c r="D498" s="26" t="s">
-        <v>6136</v>
+        <v>6137</v>
       </c>
     </row>
     <row r="499">
@@ -55666,7 +55686,7 @@
         <v>2291</v>
       </c>
       <c r="D500" s="54" t="s">
-        <v>6137</v>
+        <v>6138</v>
       </c>
     </row>
     <row r="501">
@@ -55876,7 +55896,7 @@
         <v>2363</v>
       </c>
       <c r="D515" s="54" t="s">
-        <v>6138</v>
+        <v>6139</v>
       </c>
     </row>
     <row r="516">
@@ -55890,7 +55910,7 @@
         <v>2366</v>
       </c>
       <c r="D516" s="54" t="s">
-        <v>6139</v>
+        <v>6140</v>
       </c>
     </row>
     <row r="517">
@@ -55904,7 +55924,7 @@
         <v>2369</v>
       </c>
       <c r="D517" s="54" t="s">
-        <v>6140</v>
+        <v>6141</v>
       </c>
     </row>
     <row r="518">
@@ -55918,7 +55938,7 @@
         <v>2372</v>
       </c>
       <c r="D518" s="54" t="s">
-        <v>6141</v>
+        <v>6142</v>
       </c>
     </row>
     <row r="519">
@@ -55932,7 +55952,7 @@
         <v>2375</v>
       </c>
       <c r="D519" s="54" t="s">
-        <v>6142</v>
+        <v>6143</v>
       </c>
     </row>
     <row r="520">
@@ -55974,7 +55994,7 @@
         <v>2387</v>
       </c>
       <c r="D522" s="54" t="s">
-        <v>6143</v>
+        <v>6144</v>
       </c>
     </row>
     <row r="523">
@@ -56394,7 +56414,7 @@
         <v>2523</v>
       </c>
       <c r="D552" s="54" t="s">
-        <v>6144</v>
+        <v>6145</v>
       </c>
     </row>
     <row r="553">
@@ -56450,7 +56470,7 @@
         <v>2532</v>
       </c>
       <c r="D556" s="54" t="s">
-        <v>6145</v>
+        <v>6146</v>
       </c>
     </row>
     <row r="557">
@@ -56716,7 +56736,7 @@
         <v>2632</v>
       </c>
       <c r="D575" s="22" t="s">
-        <v>6146</v>
+        <v>6147</v>
       </c>
     </row>
     <row r="576">
@@ -56786,7 +56806,7 @@
         <v>2657</v>
       </c>
       <c r="D580" s="54" t="s">
-        <v>6147</v>
+        <v>6148</v>
       </c>
     </row>
     <row r="581">
@@ -56926,7 +56946,7 @@
         <v>2701</v>
       </c>
       <c r="D590" s="54" t="s">
-        <v>6148</v>
+        <v>6149</v>
       </c>
     </row>
     <row r="591">
@@ -56940,7 +56960,7 @@
         <v>2704</v>
       </c>
       <c r="D591" s="68" t="s">
-        <v>6148</v>
+        <v>6149</v>
       </c>
     </row>
     <row r="592">
@@ -57234,7 +57254,7 @@
         <v>2793</v>
       </c>
       <c r="D612" s="54" t="s">
-        <v>6149</v>
+        <v>6150</v>
       </c>
     </row>
     <row r="613">
@@ -57273,7 +57293,7 @@
         <v>2802</v>
       </c>
       <c r="C615" s="27" t="s">
-        <v>6150</v>
+        <v>6151</v>
       </c>
       <c r="D615" s="22" t="s">
         <v>2805</v>
@@ -57444,7 +57464,7 @@
         <v>2857</v>
       </c>
       <c r="D627" s="54" t="s">
-        <v>6151</v>
+        <v>6152</v>
       </c>
     </row>
     <row r="628">
@@ -57458,7 +57478,7 @@
         <v>2860</v>
       </c>
       <c r="D628" s="54" t="s">
-        <v>6151</v>
+        <v>6152</v>
       </c>
     </row>
     <row r="629">
@@ -57500,7 +57520,7 @@
         <v>2872</v>
       </c>
       <c r="D631" s="68" t="s">
-        <v>6152</v>
+        <v>6153</v>
       </c>
     </row>
     <row r="632">
@@ -57514,7 +57534,7 @@
         <v>2874</v>
       </c>
       <c r="D632" s="54" t="s">
-        <v>6153</v>
+        <v>6154</v>
       </c>
     </row>
     <row r="633">
@@ -57738,7 +57758,7 @@
         <v>2948</v>
       </c>
       <c r="D648" s="49" t="s">
-        <v>6154</v>
+        <v>6155</v>
       </c>
     </row>
     <row r="649">
@@ -57864,7 +57884,7 @@
         <v>2987</v>
       </c>
       <c r="D657" s="49" t="s">
-        <v>6155</v>
+        <v>6156</v>
       </c>
     </row>
     <row r="658">
@@ -57892,7 +57912,7 @@
         <v>2976</v>
       </c>
       <c r="D659" s="54" t="s">
-        <v>6156</v>
+        <v>6157</v>
       </c>
     </row>
     <row r="660">
@@ -57990,7 +58010,7 @@
         <v>3022</v>
       </c>
       <c r="D666" s="58" t="s">
-        <v>6157</v>
+        <v>6158</v>
       </c>
     </row>
     <row r="667">
@@ -58004,7 +58024,7 @@
         <v>3026</v>
       </c>
       <c r="D667" s="49" t="s">
-        <v>6158</v>
+        <v>6159</v>
       </c>
     </row>
     <row r="668">
@@ -58018,7 +58038,7 @@
         <v>3028</v>
       </c>
       <c r="D668" s="49" t="s">
-        <v>6158</v>
+        <v>6159</v>
       </c>
     </row>
     <row r="669">
@@ -58088,7 +58108,7 @@
         <v>3053</v>
       </c>
       <c r="D673" s="49" t="s">
-        <v>6159</v>
+        <v>6160</v>
       </c>
     </row>
     <row r="674">
@@ -58200,7 +58220,7 @@
         <v>3085</v>
       </c>
       <c r="D681" s="49" t="s">
-        <v>6160</v>
+        <v>6161</v>
       </c>
     </row>
     <row r="682">
@@ -58214,7 +58234,7 @@
         <v>3088</v>
       </c>
       <c r="D682" s="54" t="s">
-        <v>6161</v>
+        <v>6162</v>
       </c>
     </row>
     <row r="683">
@@ -58228,7 +58248,7 @@
         <v>3091</v>
       </c>
       <c r="D683" s="54" t="s">
-        <v>6162</v>
+        <v>6163</v>
       </c>
     </row>
     <row r="684">
@@ -58320,10 +58340,10 @@
         <v>72</v>
       </c>
       <c r="B690" s="22" t="s">
-        <v>6163</v>
+        <v>6164</v>
       </c>
       <c r="C690" s="27" t="s">
-        <v>6164</v>
+        <v>6165</v>
       </c>
       <c r="D690" s="22" t="s">
         <v>3126</v>
@@ -58348,10 +58368,10 @@
         <v>72</v>
       </c>
       <c r="B692" s="22" t="s">
-        <v>6165</v>
+        <v>6166</v>
       </c>
       <c r="C692" s="22" t="s">
-        <v>6166</v>
+        <v>6167</v>
       </c>
       <c r="D692" s="22" t="s">
         <v>3137</v>
@@ -58606,7 +58626,7 @@
         <v>3229</v>
       </c>
       <c r="D710" s="57" t="s">
-        <v>6167</v>
+        <v>6168</v>
       </c>
     </row>
     <row r="711">
@@ -58620,7 +58640,7 @@
         <v>3232</v>
       </c>
       <c r="D711" s="57" t="s">
-        <v>6168</v>
+        <v>6169</v>
       </c>
     </row>
     <row r="712">
@@ -58648,7 +58668,7 @@
         <v>3236</v>
       </c>
       <c r="D713" s="49" t="s">
-        <v>6169</v>
+        <v>6170</v>
       </c>
     </row>
     <row r="714">
@@ -58956,7 +58976,7 @@
         <v>3323</v>
       </c>
       <c r="D735" s="49" t="s">
-        <v>6170</v>
+        <v>6171</v>
       </c>
     </row>
     <row r="736">
@@ -58978,10 +58998,10 @@
         <v>72</v>
       </c>
       <c r="B737" s="22" t="s">
-        <v>6171</v>
+        <v>6172</v>
       </c>
       <c r="C737" s="22" t="s">
-        <v>6172</v>
+        <v>6173</v>
       </c>
       <c r="D737" s="48" t="s">
         <v>3338</v>
@@ -59194,7 +59214,7 @@
         <v>3397</v>
       </c>
       <c r="D752" s="49" t="s">
-        <v>6173</v>
+        <v>6174</v>
       </c>
     </row>
     <row r="753">
@@ -59300,10 +59320,10 @@
         <v>72</v>
       </c>
       <c r="B760" s="22" t="s">
-        <v>6174</v>
+        <v>6175</v>
       </c>
       <c r="C760" s="22" t="s">
-        <v>6175</v>
+        <v>6176</v>
       </c>
       <c r="D760" s="48" t="s">
         <v>3470</v>
@@ -59328,10 +59348,10 @@
         <v>72</v>
       </c>
       <c r="B762" s="22" t="s">
-        <v>6176</v>
+        <v>6177</v>
       </c>
       <c r="C762" s="27" t="s">
-        <v>6176</v>
+        <v>6177</v>
       </c>
       <c r="D762" s="49" t="s">
         <v>5438</v>
@@ -59342,10 +59362,10 @@
         <v>7</v>
       </c>
       <c r="B763" s="22" t="s">
-        <v>6177</v>
+        <v>6178</v>
       </c>
       <c r="C763" s="22" t="s">
-        <v>6178</v>
+        <v>6179</v>
       </c>
       <c r="D763" s="48" t="s">
         <v>3458</v>
@@ -59356,10 +59376,10 @@
         <v>72</v>
       </c>
       <c r="B764" s="22" t="s">
-        <v>6179</v>
+        <v>6180</v>
       </c>
       <c r="C764" s="22" t="s">
-        <v>6180</v>
+        <v>6181</v>
       </c>
       <c r="D764" s="48" t="s">
         <v>3464</v>
@@ -59390,7 +59410,7 @@
         <v>3478</v>
       </c>
       <c r="D766" s="49" t="s">
-        <v>6181</v>
+        <v>6182</v>
       </c>
     </row>
     <row r="767">
@@ -59398,10 +59418,10 @@
         <v>7</v>
       </c>
       <c r="B767" s="22" t="s">
-        <v>6182</v>
+        <v>6183</v>
       </c>
       <c r="C767" s="22" t="s">
-        <v>6183</v>
+        <v>6184</v>
       </c>
       <c r="D767" s="48" t="s">
         <v>3485</v>
@@ -59412,10 +59432,10 @@
         <v>7</v>
       </c>
       <c r="B768" s="22" t="s">
-        <v>6184</v>
+        <v>6185</v>
       </c>
       <c r="C768" s="22" t="s">
-        <v>6185</v>
+        <v>6186</v>
       </c>
       <c r="D768" s="48" t="s">
         <v>3491</v>
@@ -59426,10 +59446,10 @@
         <v>53</v>
       </c>
       <c r="B769" s="22" t="s">
-        <v>6186</v>
+        <v>6187</v>
       </c>
       <c r="C769" s="22" t="s">
-        <v>6187</v>
+        <v>6188</v>
       </c>
       <c r="D769" s="48" t="s">
         <v>3497</v>
@@ -59440,10 +59460,10 @@
         <v>72</v>
       </c>
       <c r="B770" s="22" t="s">
-        <v>6188</v>
+        <v>6189</v>
       </c>
       <c r="C770" s="22" t="s">
-        <v>6189</v>
+        <v>6190</v>
       </c>
       <c r="D770" s="48" t="s">
         <v>3503</v>
@@ -59454,10 +59474,10 @@
         <v>28</v>
       </c>
       <c r="B771" s="22" t="s">
-        <v>6190</v>
+        <v>6191</v>
       </c>
       <c r="C771" s="22" t="s">
-        <v>6191</v>
+        <v>6192</v>
       </c>
       <c r="D771" s="48" t="s">
         <v>3512</v>
@@ -59468,10 +59488,10 @@
         <v>72</v>
       </c>
       <c r="B772" s="22" t="s">
-        <v>6192</v>
+        <v>6193</v>
       </c>
       <c r="C772" s="22" t="s">
-        <v>6193</v>
+        <v>6194</v>
       </c>
       <c r="D772" s="48" t="s">
         <v>3518</v>
@@ -59538,10 +59558,10 @@
         <v>53</v>
       </c>
       <c r="B777" s="22" t="s">
-        <v>6194</v>
+        <v>6195</v>
       </c>
       <c r="C777" s="22" t="s">
-        <v>6195</v>
+        <v>6196</v>
       </c>
       <c r="D777" s="48" t="s">
         <v>3547</v>
@@ -59552,10 +59572,10 @@
         <v>7</v>
       </c>
       <c r="B778" s="22" t="s">
-        <v>6196</v>
+        <v>6197</v>
       </c>
       <c r="C778" s="22" t="s">
-        <v>6197</v>
+        <v>6198</v>
       </c>
       <c r="D778" s="48" t="s">
         <v>3553</v>
@@ -59566,10 +59586,10 @@
         <v>7</v>
       </c>
       <c r="B779" s="22" t="s">
-        <v>6198</v>
+        <v>6199</v>
       </c>
       <c r="C779" s="22" t="s">
-        <v>6199</v>
+        <v>6200</v>
       </c>
       <c r="D779" s="48" t="s">
         <v>3559</v>
@@ -59580,10 +59600,10 @@
         <v>72</v>
       </c>
       <c r="B780" s="22" t="s">
-        <v>6200</v>
+        <v>6201</v>
       </c>
       <c r="C780" s="22" t="s">
-        <v>6201</v>
+        <v>6202</v>
       </c>
       <c r="D780" s="48" t="s">
         <v>3565</v>
@@ -59594,10 +59614,10 @@
         <v>72</v>
       </c>
       <c r="B781" s="22" t="s">
-        <v>6202</v>
+        <v>6203</v>
       </c>
       <c r="C781" s="22" t="s">
-        <v>6203</v>
+        <v>6204</v>
       </c>
       <c r="D781" s="48" t="s">
         <v>3571</v>
@@ -59622,10 +59642,10 @@
         <v>72</v>
       </c>
       <c r="B783" s="22" t="s">
-        <v>6204</v>
+        <v>6205</v>
       </c>
       <c r="C783" s="22" t="s">
-        <v>6205</v>
+        <v>6206</v>
       </c>
       <c r="D783" s="48" t="s">
         <v>3583</v>
@@ -59636,10 +59656,10 @@
         <v>7</v>
       </c>
       <c r="B784" s="22" t="s">
-        <v>6206</v>
+        <v>6207</v>
       </c>
       <c r="C784" s="22" t="s">
-        <v>6207</v>
+        <v>6208</v>
       </c>
       <c r="D784" s="48" t="s">
         <v>3589</v>
@@ -59670,7 +59690,7 @@
         <v>3594</v>
       </c>
       <c r="D786" s="49" t="s">
-        <v>6208</v>
+        <v>6209</v>
       </c>
     </row>
     <row r="787">
@@ -59698,7 +59718,7 @@
         <v>3601</v>
       </c>
       <c r="D788" s="49" t="s">
-        <v>6209</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="789">
@@ -60076,7 +60096,7 @@
         <v>3734</v>
       </c>
       <c r="D815" s="49" t="s">
-        <v>6210</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="816">
@@ -60216,7 +60236,7 @@
         <v>2629</v>
       </c>
       <c r="D825" s="49" t="s">
-        <v>6211</v>
+        <v>6212</v>
       </c>
     </row>
     <row r="826">
@@ -60244,7 +60264,7 @@
         <v>3778</v>
       </c>
       <c r="D827" s="49" t="s">
-        <v>6212</v>
+        <v>6213</v>
       </c>
     </row>
     <row r="828">
@@ -60370,7 +60390,7 @@
         <v>3819</v>
       </c>
       <c r="D836" s="54" t="s">
-        <v>6213</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="837">
@@ -60384,7 +60404,7 @@
         <v>3822</v>
       </c>
       <c r="D837" s="54" t="s">
-        <v>6213</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="838">
@@ -60650,7 +60670,7 @@
         <v>3907</v>
       </c>
       <c r="D856" s="49" t="s">
-        <v>6214</v>
+        <v>6215</v>
       </c>
     </row>
     <row r="857">
@@ -60720,7 +60740,7 @@
         <v>3925</v>
       </c>
       <c r="D861" s="49" t="s">
-        <v>6215</v>
+        <v>6216</v>
       </c>
     </row>
     <row r="862">
@@ -60762,7 +60782,7 @@
         <v>3942</v>
       </c>
       <c r="D864" s="49" t="s">
-        <v>6216</v>
+        <v>6217</v>
       </c>
     </row>
     <row r="865">
@@ -60958,7 +60978,7 @@
         <v>3997</v>
       </c>
       <c r="D878" s="49" t="s">
-        <v>6217</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="879">
@@ -60972,7 +60992,7 @@
         <v>4000</v>
       </c>
       <c r="D879" s="49" t="s">
-        <v>6217</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="880">
@@ -60986,7 +61006,7 @@
         <v>4002</v>
       </c>
       <c r="D880" s="58" t="s">
-        <v>6218</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="881">
@@ -61000,7 +61020,7 @@
         <v>4005</v>
       </c>
       <c r="D881" s="49" t="s">
-        <v>6219</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="882">
@@ -61168,7 +61188,7 @@
         <v>4063</v>
       </c>
       <c r="D893" s="49" t="s">
-        <v>6220</v>
+        <v>6221</v>
       </c>
     </row>
     <row r="894">
@@ -61176,10 +61196,10 @@
         <v>72</v>
       </c>
       <c r="B894" s="22" t="s">
-        <v>6221</v>
+        <v>6222</v>
       </c>
       <c r="C894" s="52" t="s">
-        <v>6222</v>
+        <v>6223</v>
       </c>
       <c r="D894" s="48" t="s">
         <v>4070</v>
@@ -61190,10 +61210,10 @@
         <v>105</v>
       </c>
       <c r="B895" s="22" t="s">
-        <v>6223</v>
+        <v>6224</v>
       </c>
       <c r="C895" s="22" t="s">
-        <v>6224</v>
+        <v>6225</v>
       </c>
       <c r="D895" s="48" t="s">
         <v>917</v>
@@ -61224,7 +61244,7 @@
         <v>4077</v>
       </c>
       <c r="D897" s="49" t="s">
-        <v>6225</v>
+        <v>6226</v>
       </c>
     </row>
     <row r="898">
@@ -61238,7 +61258,7 @@
         <v>4081</v>
       </c>
       <c r="D898" s="49" t="s">
-        <v>6226</v>
+        <v>6227</v>
       </c>
     </row>
     <row r="899">
@@ -61406,7 +61426,7 @@
         <v>4145</v>
       </c>
       <c r="D910" s="49" t="s">
-        <v>6227</v>
+        <v>6228</v>
       </c>
     </row>
     <row r="911">
@@ -62072,7 +62092,7 @@
         <v>72</v>
       </c>
       <c r="B958" s="22" t="s">
-        <v>6228</v>
+        <v>6229</v>
       </c>
       <c r="C958" s="22" t="s">
         <v>4911</v>
@@ -62456,7 +62476,7 @@
         <v>4510</v>
       </c>
       <c r="D985" s="49" t="s">
-        <v>6229</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="986">
@@ -62512,7 +62532,7 @@
         <v>4529</v>
       </c>
       <c r="D989" s="49" t="s">
-        <v>6230</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="990">
@@ -62568,7 +62588,7 @@
         <v>4544</v>
       </c>
       <c r="D993" s="49" t="s">
-        <v>6231</v>
+        <v>6232</v>
       </c>
     </row>
     <row r="994">
@@ -62582,7 +62602,7 @@
         <v>4547</v>
       </c>
       <c r="D994" s="49" t="s">
-        <v>6231</v>
+        <v>6232</v>
       </c>
     </row>
     <row r="995">
@@ -62610,7 +62630,7 @@
         <v>4554</v>
       </c>
       <c r="D996" s="49" t="s">
-        <v>6232</v>
+        <v>6233</v>
       </c>
     </row>
     <row r="997">
@@ -62666,7 +62686,7 @@
         <v>4567</v>
       </c>
       <c r="D1000" s="49" t="s">
-        <v>6233</v>
+        <v>6234</v>
       </c>
     </row>
     <row r="1001">
@@ -62680,7 +62700,7 @@
         <v>4571</v>
       </c>
       <c r="D1001" s="49" t="s">
-        <v>6234</v>
+        <v>6235</v>
       </c>
     </row>
     <row r="1002">
@@ -62694,7 +62714,7 @@
         <v>4577</v>
       </c>
       <c r="D1002" s="49" t="s">
-        <v>6235</v>
+        <v>6236</v>
       </c>
     </row>
     <row r="1003">
@@ -62722,7 +62742,7 @@
         <v>4601</v>
       </c>
       <c r="D1004" s="49" t="s">
-        <v>6236</v>
+        <v>6237</v>
       </c>
     </row>
     <row r="1005">
@@ -62736,7 +62756,7 @@
         <v>4612</v>
       </c>
       <c r="D1005" s="49" t="s">
-        <v>6237</v>
+        <v>6238</v>
       </c>
     </row>
     <row r="1006">
@@ -62764,7 +62784,7 @@
         <v>4630</v>
       </c>
       <c r="D1007" s="49" t="s">
-        <v>6146</v>
+        <v>6147</v>
       </c>
     </row>
     <row r="1008">
@@ -62778,7 +62798,7 @@
         <v>4645</v>
       </c>
       <c r="D1008" s="49" t="s">
-        <v>6238</v>
+        <v>6239</v>
       </c>
     </row>
     <row r="1009">
@@ -62806,7 +62826,7 @@
         <v>4656</v>
       </c>
       <c r="D1010" s="49" t="s">
-        <v>6239</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="1011">
@@ -62834,7 +62854,7 @@
         <v>4601</v>
       </c>
       <c r="D1012" s="49" t="s">
-        <v>6236</v>
+        <v>6237</v>
       </c>
     </row>
     <row r="1013">
@@ -62918,7 +62938,7 @@
         <v>4696</v>
       </c>
       <c r="D1018" s="49" t="s">
-        <v>6240</v>
+        <v>6241</v>
       </c>
     </row>
     <row r="1019">
@@ -63030,7 +63050,7 @@
         <v>4736</v>
       </c>
       <c r="D1026" s="49" t="s">
-        <v>6241</v>
+        <v>6242</v>
       </c>
     </row>
     <row r="1027">
@@ -63044,7 +63064,7 @@
         <v>4741</v>
       </c>
       <c r="D1027" s="49" t="s">
-        <v>6242</v>
+        <v>6243</v>
       </c>
     </row>
     <row r="1028">
@@ -63058,7 +63078,7 @@
         <v>4739</v>
       </c>
       <c r="D1028" s="49" t="s">
-        <v>6243</v>
+        <v>6244</v>
       </c>
     </row>
     <row r="1029">
@@ -63251,7 +63271,7 @@
         <v>4807</v>
       </c>
       <c r="C1042" s="52" t="s">
-        <v>6244</v>
+        <v>6245</v>
       </c>
       <c r="D1042" s="48" t="s">
         <v>4810</v>
@@ -63520,7 +63540,7 @@
         <v>4917</v>
       </c>
       <c r="D1061" s="49" t="s">
-        <v>6245</v>
+        <v>6246</v>
       </c>
     </row>
     <row r="1062">
@@ -63534,7 +63554,7 @@
         <v>4920</v>
       </c>
       <c r="D1062" s="49" t="s">
-        <v>6245</v>
+        <v>6246</v>
       </c>
     </row>
     <row r="1063">
@@ -63618,7 +63638,7 @@
         <v>4947</v>
       </c>
       <c r="D1068" s="49" t="s">
-        <v>6246</v>
+        <v>6247</v>
       </c>
     </row>
     <row r="1069">
@@ -63685,10 +63705,10 @@
         <v>4971</v>
       </c>
       <c r="C1073" s="22" t="s">
-        <v>6247</v>
+        <v>6248</v>
       </c>
       <c r="D1073" s="49" t="s">
-        <v>6248</v>
+        <v>6249</v>
       </c>
     </row>
     <row r="1074">
@@ -63699,10 +63719,10 @@
         <v>4976</v>
       </c>
       <c r="C1074" s="22" t="s">
-        <v>6249</v>
+        <v>6250</v>
       </c>
       <c r="D1074" s="49" t="s">
-        <v>6250</v>
+        <v>6251</v>
       </c>
     </row>
     <row r="1075">
@@ -63724,10 +63744,10 @@
         <v>72</v>
       </c>
       <c r="B1076" s="22" t="s">
-        <v>6251</v>
+        <v>6252</v>
       </c>
       <c r="C1076" s="22" t="s">
-        <v>6252</v>
+        <v>6253</v>
       </c>
       <c r="D1076" s="48" t="s">
         <v>2822</v>
@@ -63884,7 +63904,7 @@
         <v>5034</v>
       </c>
       <c r="D1087" s="49" t="s">
-        <v>6253</v>
+        <v>6254</v>
       </c>
     </row>
     <row r="1088">
@@ -63926,7 +63946,7 @@
         <v>5049</v>
       </c>
       <c r="D1090" s="49" t="s">
-        <v>6254</v>
+        <v>6255</v>
       </c>
     </row>
     <row r="1091">
@@ -63968,7 +63988,7 @@
         <v>5057</v>
       </c>
       <c r="D1093" s="49" t="s">
-        <v>6255</v>
+        <v>6256</v>
       </c>
     </row>
     <row r="1094">
@@ -64038,7 +64058,7 @@
         <v>5080</v>
       </c>
       <c r="D1098" s="49" t="s">
-        <v>6256</v>
+        <v>6257</v>
       </c>
     </row>
     <row r="1099">
@@ -64108,7 +64128,7 @@
         <v>5101</v>
       </c>
       <c r="D1103" s="49" t="s">
-        <v>6257</v>
+        <v>6258</v>
       </c>
     </row>
     <row r="1104">
@@ -64122,7 +64142,7 @@
         <v>5107</v>
       </c>
       <c r="D1104" s="49" t="s">
-        <v>6258</v>
+        <v>6259</v>
       </c>
     </row>
     <row r="1105">
@@ -64136,7 +64156,7 @@
         <v>5113</v>
       </c>
       <c r="D1105" s="54" t="s">
-        <v>6259</v>
+        <v>6260</v>
       </c>
     </row>
     <row r="1106">
@@ -64150,7 +64170,7 @@
         <v>5117</v>
       </c>
       <c r="D1106" s="62" t="s">
-        <v>6260</v>
+        <v>6261</v>
       </c>
     </row>
     <row r="1107">
@@ -64248,7 +64268,7 @@
         <v>5154</v>
       </c>
       <c r="D1113" s="49" t="s">
-        <v>6261</v>
+        <v>6262</v>
       </c>
     </row>
     <row r="1114">
@@ -64262,7 +64282,7 @@
         <v>5159</v>
       </c>
       <c r="D1114" s="49" t="s">
-        <v>6262</v>
+        <v>6263</v>
       </c>
     </row>
     <row r="1115">
@@ -64584,7 +64604,7 @@
         <v>5262</v>
       </c>
       <c r="D1137" s="62" t="s">
-        <v>6263</v>
+        <v>6264</v>
       </c>
     </row>
     <row r="1138">
@@ -64640,7 +64660,7 @@
         <v>5281</v>
       </c>
       <c r="D1141" s="49" t="s">
-        <v>6264</v>
+        <v>6265</v>
       </c>
     </row>
     <row r="1142">
@@ -64654,7 +64674,7 @@
         <v>5284</v>
       </c>
       <c r="D1142" s="49" t="s">
-        <v>6264</v>
+        <v>6265</v>
       </c>
     </row>
     <row r="1143">
@@ -64668,7 +64688,7 @@
         <v>5286</v>
       </c>
       <c r="D1143" s="49" t="s">
-        <v>6265</v>
+        <v>6266</v>
       </c>
     </row>
     <row r="1144">
@@ -64738,7 +64758,7 @@
         <v>5303</v>
       </c>
       <c r="D1148" s="49" t="s">
-        <v>6266</v>
+        <v>6267</v>
       </c>
     </row>
     <row r="1149">
@@ -64920,7 +64940,7 @@
         <v>5358</v>
       </c>
       <c r="D1161" s="49" t="s">
-        <v>6267</v>
+        <v>6268</v>
       </c>
     </row>
     <row r="1162">
@@ -64934,7 +64954,7 @@
         <v>5362</v>
       </c>
       <c r="D1162" s="49" t="s">
-        <v>6268</v>
+        <v>6269</v>
       </c>
     </row>
     <row r="1163">
@@ -65004,7 +65024,7 @@
         <v>5387</v>
       </c>
       <c r="D1167" s="54" t="s">
-        <v>6269</v>
+        <v>6270</v>
       </c>
     </row>
     <row r="1168">
@@ -65200,7 +65220,7 @@
         <v>5453</v>
       </c>
       <c r="D1181" s="49" t="s">
-        <v>6270</v>
+        <v>6271</v>
       </c>
     </row>
     <row r="1182">
@@ -65214,7 +65234,7 @@
         <v>5455</v>
       </c>
       <c r="D1182" s="49" t="s">
-        <v>6271</v>
+        <v>6272</v>
       </c>
     </row>
     <row r="1183">
@@ -65228,7 +65248,7 @@
         <v>5458</v>
       </c>
       <c r="D1183" s="62" t="s">
-        <v>6272</v>
+        <v>6273</v>
       </c>
     </row>
     <row r="1184">
@@ -65256,7 +65276,7 @@
         <v>5463</v>
       </c>
       <c r="D1185" s="49" t="s">
-        <v>6273</v>
+        <v>6274</v>
       </c>
     </row>
     <row r="1186">
@@ -65284,7 +65304,7 @@
         <v>5468</v>
       </c>
       <c r="D1187" s="49" t="s">
-        <v>6274</v>
+        <v>6275</v>
       </c>
     </row>
     <row r="1188">
@@ -65312,7 +65332,7 @@
         <v>5473</v>
       </c>
       <c r="D1189" s="49" t="s">
-        <v>6275</v>
+        <v>6276</v>
       </c>
     </row>
     <row r="1190">
@@ -65452,7 +65472,7 @@
         <v>5512</v>
       </c>
       <c r="D1199" s="49" t="s">
-        <v>6276</v>
+        <v>6277</v>
       </c>
     </row>
     <row r="1200">
@@ -65522,7 +65542,7 @@
         <v>5534</v>
       </c>
       <c r="D1204" s="49" t="s">
-        <v>6277</v>
+        <v>6278</v>
       </c>
     </row>
     <row r="1205">
@@ -65533,10 +65553,10 @@
         <v>5538</v>
       </c>
       <c r="C1205" s="22" t="s">
-        <v>6278</v>
+        <v>6279</v>
       </c>
       <c r="D1205" s="49" t="s">
-        <v>6279</v>
+        <v>6280</v>
       </c>
     </row>
     <row r="1206">
@@ -65564,7 +65584,7 @@
         <v>5549</v>
       </c>
       <c r="D1207" s="49" t="s">
-        <v>6280</v>
+        <v>6281</v>
       </c>
     </row>
     <row r="1208">
@@ -65757,7 +65777,7 @@
         <v>5609</v>
       </c>
       <c r="C1221" s="22" t="s">
-        <v>6281</v>
+        <v>6282</v>
       </c>
       <c r="D1221" s="48" t="s">
         <v>5612</v>
@@ -65774,7 +65794,7 @@
         <v>5614</v>
       </c>
       <c r="D1222" s="58" t="s">
-        <v>6282</v>
+        <v>6283</v>
       </c>
     </row>
     <row r="1223">
@@ -65928,7 +65948,7 @@
         <v>5661</v>
       </c>
       <c r="D1233" s="49" t="s">
-        <v>6283</v>
+        <v>6284</v>
       </c>
     </row>
     <row r="1234">
@@ -66068,7 +66088,7 @@
         <v>5697</v>
       </c>
       <c r="D1243" s="49" t="s">
-        <v>6284</v>
+        <v>6285</v>
       </c>
     </row>
     <row r="1244">
@@ -66180,7 +66200,7 @@
         <v>5739</v>
       </c>
       <c r="D1251" s="49" t="s">
-        <v>6285</v>
+        <v>6286</v>
       </c>
     </row>
     <row r="1252">
@@ -66558,7 +66578,7 @@
         <v>5473</v>
       </c>
       <c r="D1278" s="49" t="s">
-        <v>6275</v>
+        <v>6276</v>
       </c>
     </row>
     <row r="1279">
@@ -66572,7 +66592,7 @@
         <v>5881</v>
       </c>
       <c r="D1279" s="49" t="s">
-        <v>6286</v>
+        <v>6287</v>
       </c>
     </row>
     <row r="1280">
@@ -66726,7 +66746,7 @@
         <v>5934</v>
       </c>
       <c r="D1290" s="49" t="s">
-        <v>6287</v>
+        <v>6288</v>
       </c>
     </row>
     <row r="1291">
@@ -66964,7 +66984,7 @@
         <v>6018</v>
       </c>
       <c r="D1307" s="54" t="s">
-        <v>6288</v>
+        <v>6289</v>
       </c>
     </row>
     <row r="1308">
@@ -67000,13 +67020,13 @@
         <v>53</v>
       </c>
       <c r="B1310" s="22" t="s">
-        <v>6032</v>
+        <v>6034</v>
       </c>
       <c r="C1310" s="27" t="s">
-        <v>6032</v>
+        <v>6034</v>
       </c>
       <c r="D1310" s="22" t="s">
-        <v>6035</v>
+        <v>6036</v>
       </c>
     </row>
     <row r="1311">
@@ -67014,13 +67034,13 @@
         <v>53</v>
       </c>
       <c r="B1311" s="22" t="s">
-        <v>6036</v>
+        <v>6037</v>
       </c>
       <c r="C1311" s="27" t="s">
-        <v>6037</v>
+        <v>6038</v>
       </c>
       <c r="D1311" s="22" t="s">
-        <v>6041</v>
+        <v>6042</v>
       </c>
     </row>
     <row r="1312">
@@ -67028,13 +67048,13 @@
         <v>105</v>
       </c>
       <c r="B1312" s="22" t="s">
-        <v>6042</v>
+        <v>6043</v>
       </c>
       <c r="C1312" s="27" t="s">
-        <v>6043</v>
+        <v>6044</v>
       </c>
       <c r="D1312" s="22" t="s">
-        <v>6045</v>
+        <v>6046</v>
       </c>
     </row>
     <row r="1313">
@@ -67042,13 +67062,13 @@
         <v>72</v>
       </c>
       <c r="B1313" s="22" t="s">
-        <v>6046</v>
+        <v>6047</v>
       </c>
       <c r="C1313" s="27" t="s">
-        <v>6047</v>
+        <v>6048</v>
       </c>
       <c r="D1313" s="22" t="s">
-        <v>6049</v>
+        <v>6050</v>
       </c>
     </row>
     <row r="1314">
@@ -67056,13 +67076,13 @@
         <v>105</v>
       </c>
       <c r="B1314" s="22" t="s">
-        <v>6050</v>
+        <v>6051</v>
       </c>
       <c r="C1314" s="27" t="s">
-        <v>6051</v>
+        <v>6052</v>
       </c>
       <c r="D1314" s="22" t="s">
-        <v>6052</v>
+        <v>6053</v>
       </c>
     </row>
     <row r="1315">
@@ -67070,13 +67090,13 @@
         <v>105</v>
       </c>
       <c r="B1315" s="22" t="s">
-        <v>6053</v>
+        <v>6054</v>
       </c>
       <c r="C1315" s="27" t="s">
-        <v>6054</v>
+        <v>6055</v>
       </c>
       <c r="D1315" s="22" t="s">
-        <v>6056</v>
+        <v>6057</v>
       </c>
     </row>
     <row r="1316">
@@ -67084,13 +67104,13 @@
         <v>105</v>
       </c>
       <c r="B1316" s="22" t="s">
-        <v>6057</v>
+        <v>6058</v>
       </c>
       <c r="C1316" s="27" t="s">
-        <v>6058</v>
+        <v>6059</v>
       </c>
       <c r="D1316" s="22" t="s">
-        <v>6059</v>
+        <v>6060</v>
       </c>
     </row>
     <row r="1317">
@@ -67104,7 +67124,7 @@
         <v>3194</v>
       </c>
       <c r="D1317" s="54" t="s">
-        <v>6289</v>
+        <v>6290</v>
       </c>
     </row>
     <row r="1318">
@@ -67118,7 +67138,7 @@
         <v>3200</v>
       </c>
       <c r="D1318" s="54" t="s">
-        <v>6290</v>
+        <v>6291</v>
       </c>
     </row>
     <row r="1319">
@@ -67132,7 +67152,7 @@
         <v>5129</v>
       </c>
       <c r="D1319" s="54" t="s">
-        <v>6291</v>
+        <v>6292</v>
       </c>
     </row>
     <row r="1320">
@@ -67146,7 +67166,7 @@
         <v>2629</v>
       </c>
       <c r="D1320" s="54" t="s">
-        <v>6292</v>
+        <v>6293</v>
       </c>
     </row>
     <row r="1321">
@@ -67160,7 +67180,7 @@
         <v>1902</v>
       </c>
       <c r="D1321" s="54" t="s">
-        <v>6293</v>
+        <v>6294</v>
       </c>
     </row>
     <row r="1322">
@@ -67174,7 +67194,7 @@
         <v>156</v>
       </c>
       <c r="D1322" s="54" t="s">
-        <v>6294</v>
+        <v>6295</v>
       </c>
     </row>
     <row r="1323">
@@ -67188,7 +67208,7 @@
         <v>485</v>
       </c>
       <c r="D1323" s="54" t="s">
-        <v>6295</v>
+        <v>6296</v>
       </c>
     </row>
     <row r="1324">
@@ -67202,7 +67222,7 @@
         <v>4642</v>
       </c>
       <c r="D1324" s="54" t="s">
-        <v>6296</v>
+        <v>6297</v>
       </c>
     </row>
     <row r="1325">
@@ -67216,7 +67236,7 @@
         <v>4606</v>
       </c>
       <c r="D1325" s="54" t="s">
-        <v>6297</v>
+        <v>6298</v>
       </c>
     </row>
     <row r="1326">
@@ -67230,7 +67250,7 @@
         <v>4167</v>
       </c>
       <c r="D1326" s="54" t="s">
-        <v>6298</v>
+        <v>6299</v>
       </c>
     </row>
     <row r="1327">
@@ -67244,7 +67264,7 @@
         <v>4501</v>
       </c>
       <c r="D1327" s="54" t="s">
-        <v>6299</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="1328">
@@ -67258,7 +67278,7 @@
         <v>4201</v>
       </c>
       <c r="D1328" s="54" t="s">
-        <v>6300</v>
+        <v>6301</v>
       </c>
     </row>
     <row r="1329">
@@ -67286,7 +67306,7 @@
         <v>3013</v>
       </c>
       <c r="D1330" s="54" t="s">
-        <v>6301</v>
+        <v>6302</v>
       </c>
     </row>
     <row r="1331">
@@ -67300,7 +67320,7 @@
         <v>3649</v>
       </c>
       <c r="D1331" s="54" t="s">
-        <v>6302</v>
+        <v>6303</v>
       </c>
     </row>
     <row r="1332">
@@ -67314,7 +67334,7 @@
         <v>5869</v>
       </c>
       <c r="D1332" s="54" t="s">
-        <v>6303</v>
+        <v>6304</v>
       </c>
     </row>
     <row r="1333">
@@ -67328,7 +67348,7 @@
         <v>5872</v>
       </c>
       <c r="D1333" s="54" t="s">
-        <v>6304</v>
+        <v>6305</v>
       </c>
     </row>
     <row r="1334">
@@ -67342,7 +67362,7 @@
         <v>1899</v>
       </c>
       <c r="D1334" s="54" t="s">
-        <v>6305</v>
+        <v>6306</v>
       </c>
     </row>
     <row r="1335">
@@ -67356,7 +67376,7 @@
         <v>1663</v>
       </c>
       <c r="D1335" s="54" t="s">
-        <v>6306</v>
+        <v>6307</v>
       </c>
     </row>
     <row r="1336">
@@ -67370,7 +67390,7 @@
         <v>4392</v>
       </c>
       <c r="D1336" s="54" t="s">
-        <v>6307</v>
+        <v>6308</v>
       </c>
     </row>
     <row r="1337">
@@ -67378,10 +67398,10 @@
         <v>124</v>
       </c>
       <c r="B1337" s="22" t="s">
-        <v>6308</v>
+        <v>6309</v>
       </c>
       <c r="C1337" s="27" t="s">
-        <v>6201</v>
+        <v>6202</v>
       </c>
       <c r="D1337" s="54" t="s">
         <v>3565</v>
@@ -67398,7 +67418,7 @@
         <v>5110</v>
       </c>
       <c r="D1338" s="88" t="s">
-        <v>6309</v>
+        <v>6310</v>
       </c>
     </row>
     <row r="1339">
@@ -67412,7 +67432,7 @@
         <v>3756</v>
       </c>
       <c r="D1339" s="54" t="s">
-        <v>6310</v>
+        <v>6311</v>
       </c>
     </row>
     <row r="1340">
@@ -67426,7 +67446,7 @@
         <v>1957</v>
       </c>
       <c r="D1340" s="54" t="s">
-        <v>6311</v>
+        <v>6312</v>
       </c>
     </row>
     <row r="1341">
@@ -67440,7 +67460,7 @@
         <v>4292</v>
       </c>
       <c r="D1341" s="54" t="s">
-        <v>6312</v>
+        <v>6313</v>
       </c>
     </row>
     <row r="1342">
@@ -67454,7 +67474,7 @@
         <v>5423</v>
       </c>
       <c r="D1342" s="54" t="s">
-        <v>6313</v>
+        <v>6314</v>
       </c>
     </row>
     <row r="1343">
@@ -67468,7 +67488,7 @@
         <v>3737</v>
       </c>
       <c r="D1343" s="54" t="s">
-        <v>6314</v>
+        <v>6315</v>
       </c>
     </row>
     <row r="1344">
@@ -67482,7 +67502,7 @@
         <v>1131</v>
       </c>
       <c r="D1344" s="54" t="s">
-        <v>6315</v>
+        <v>6316</v>
       </c>
     </row>
     <row r="1345">
@@ -67496,7 +67516,7 @@
         <v>2713</v>
       </c>
       <c r="D1345" s="54" t="s">
-        <v>6316</v>
+        <v>6317</v>
       </c>
     </row>
     <row r="1346">
@@ -67510,7 +67530,7 @@
         <v>3426</v>
       </c>
       <c r="D1346" s="54" t="s">
-        <v>6317</v>
+        <v>6318</v>
       </c>
     </row>
     <row r="1347">
@@ -67538,7 +67558,7 @@
         <v>567</v>
       </c>
       <c r="D1348" s="54" t="s">
-        <v>6318</v>
+        <v>6319</v>
       </c>
     </row>
     <row r="1349">
@@ -67552,7 +67572,7 @@
         <v>5011</v>
       </c>
       <c r="D1349" s="54" t="s">
-        <v>6319</v>
+        <v>6320</v>
       </c>
     </row>
     <row r="1350">
@@ -67566,7 +67586,7 @@
         <v>2078</v>
       </c>
       <c r="D1350" s="54" t="s">
-        <v>6320</v>
+        <v>6321</v>
       </c>
     </row>
     <row r="1351">
@@ -67580,7 +67600,7 @@
         <v>455</v>
       </c>
       <c r="D1351" s="54" t="s">
-        <v>6321</v>
+        <v>6322</v>
       </c>
     </row>
     <row r="1352">
@@ -67594,7 +67614,7 @@
         <v>4034</v>
       </c>
       <c r="D1352" s="54" t="s">
-        <v>6322</v>
+        <v>6323</v>
       </c>
     </row>
     <row r="1353">
@@ -67636,7 +67656,7 @@
         <v>4094</v>
       </c>
       <c r="D1355" s="54" t="s">
-        <v>6323</v>
+        <v>6324</v>
       </c>
     </row>
     <row r="1356">
@@ -67650,7 +67670,7 @@
         <v>4091</v>
       </c>
       <c r="D1356" s="54" t="s">
-        <v>6324</v>
+        <v>6325</v>
       </c>
     </row>
     <row r="1357">
@@ -67664,7 +67684,7 @@
         <v>5902</v>
       </c>
       <c r="D1357" s="54" t="s">
-        <v>6325</v>
+        <v>6326</v>
       </c>
     </row>
     <row r="1358">
@@ -67692,7 +67712,7 @@
         <v>4044</v>
       </c>
       <c r="D1359" s="54" t="s">
-        <v>6326</v>
+        <v>6327</v>
       </c>
     </row>
     <row r="1360">
@@ -67706,7 +67726,7 @@
         <v>3441</v>
       </c>
       <c r="D1360" s="54" t="s">
-        <v>6327</v>
+        <v>6328</v>
       </c>
     </row>
     <row r="1361">
@@ -67720,7 +67740,7 @@
         <v>5292</v>
       </c>
       <c r="D1361" s="68" t="s">
-        <v>6328</v>
+        <v>6329</v>
       </c>
     </row>
     <row r="1362">
@@ -67734,7 +67754,7 @@
         <v>1255</v>
       </c>
       <c r="D1362" s="54" t="s">
-        <v>6329</v>
+        <v>6330</v>
       </c>
     </row>
     <row r="1363">
@@ -67748,7 +67768,7 @@
         <v>4674</v>
       </c>
       <c r="D1363" s="54" t="s">
-        <v>6330</v>
+        <v>6331</v>
       </c>
     </row>
     <row r="1364">
@@ -67776,7 +67796,7 @@
         <v>3423</v>
       </c>
       <c r="D1365" s="54" t="s">
-        <v>6331</v>
+        <v>6332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHOOSE to Choose (#97)
* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_E51826C2_77A0_49F5_A86D_C45D819E3570_.wvu.FilterData">'client strings'!$D$1:$D$1427</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_5031FDED_2F5F_443E_85C3_7F1B49A7B6E0_.wvu.FilterData">'client strings'!$C$1:$C$1427</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0EFEF162_7613_43FE_AC97_5D237109F557_.wvu.FilterData">'client strings'!$C$1:$C$1427</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_5FF530B0_04DD_454E_B0A4_4D23275EBB9F_.wvu.FilterData">'client strings'!$D$1:$D$1427</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{5031FDED-2F5F-443E-85C3-7F1B49A7B6E0}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E51826C2-77A0-49F5-A86D-C45D819E3570}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0EFEF162-7613-43FE-AC97-5D237109F557}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{5FF530B0-04DD-454E-B0A4-4D23275EBB9F}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14154" uniqueCount="6424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14154" uniqueCount="6425">
   <si>
     <t>platform</t>
   </si>
@@ -3729,7 +3729,7 @@
     <t>Memeriksa info pembayaran</t>
   </si>
   <si>
-    <t>CHOOSE</t>
+    <t>Choose</t>
   </si>
   <si>
     <t>选择</t>
@@ -19299,6 +19299,9 @@
   </si>
   <si>
     <t>Convenient wallet for popular cryptocurrencies</t>
+  </si>
+  <si>
+    <t>CHOOSE</t>
   </si>
   <si>
     <r>
@@ -25816,10 +25819,10 @@
       <c r="A266" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B266" s="4" t="s">
+      <c r="B266" s="1" t="s">
         <v>1224</v>
       </c>
-      <c r="C266" s="4" t="s">
+      <c r="C266" s="1" t="s">
         <v>1224</v>
       </c>
       <c r="D266" s="4" t="s">
@@ -50306,10 +50309,10 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E51826C2-77A0-49F5-A86D-C45D819E3570}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{5FF530B0-04DD-454E-B0A4-4D23275EBB9F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1427"/>
     </customSheetView>
-    <customSheetView guid="{5031FDED-2F5F-443E-85C3-7F1B49A7B6E0}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0EFEF162-7613-43FE-AC97-5D237109F557}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1427"/>
     </customSheetView>
   </customSheetViews>
@@ -54090,10 +54093,10 @@
         <v>7</v>
       </c>
       <c r="B266" s="27" t="s">
-        <v>1224</v>
+        <v>6406</v>
       </c>
       <c r="C266" s="27" t="s">
-        <v>1224</v>
+        <v>6406</v>
       </c>
       <c r="D266" s="52" t="s">
         <v>641</v>
@@ -54681,7 +54684,7 @@
         <v>1402</v>
       </c>
       <c r="C308" s="72" t="s">
-        <v>6406</v>
+        <v>6407</v>
       </c>
       <c r="D308" s="51" t="s">
         <v>1405</v>
@@ -59780,7 +59783,7 @@
         <v>3051</v>
       </c>
       <c r="D672" s="85" t="s">
-        <v>6407</v>
+        <v>6408</v>
       </c>
     </row>
     <row r="673">
@@ -61930,10 +61933,10 @@
         <v>169</v>
       </c>
       <c r="B826" s="27" t="s">
-        <v>6408</v>
+        <v>6409</v>
       </c>
       <c r="C826" s="27" t="s">
-        <v>6409</v>
+        <v>6410</v>
       </c>
       <c r="D826" s="51" t="s">
         <v>3741</v>
@@ -63882,7 +63885,7 @@
         <v>4341</v>
       </c>
       <c r="D965" s="51" t="s">
-        <v>6410</v>
+        <v>6411</v>
       </c>
     </row>
     <row r="966">
@@ -65268,7 +65271,7 @@
         <v>4788</v>
       </c>
       <c r="D1064" s="51" t="s">
-        <v>6411</v>
+        <v>6412</v>
       </c>
     </row>
     <row r="1065">
@@ -65296,7 +65299,7 @@
         <v>4796</v>
       </c>
       <c r="D1066" s="51" t="s">
-        <v>6412</v>
+        <v>6413</v>
       </c>
     </row>
     <row r="1067">
@@ -65324,7 +65327,7 @@
         <v>4804</v>
       </c>
       <c r="D1068" s="51" t="s">
-        <v>6413</v>
+        <v>6414</v>
       </c>
     </row>
     <row r="1069">
@@ -65366,7 +65369,7 @@
         <v>4816</v>
       </c>
       <c r="D1071" s="52" t="s">
-        <v>6414</v>
+        <v>6415</v>
       </c>
     </row>
     <row r="1072">
@@ -65436,7 +65439,7 @@
         <v>4836</v>
       </c>
       <c r="D1076" s="61" t="s">
-        <v>6415</v>
+        <v>6416</v>
       </c>
     </row>
     <row r="1077">
@@ -65478,7 +65481,7 @@
         <v>4850</v>
       </c>
       <c r="D1079" s="51" t="s">
-        <v>6416</v>
+        <v>6417</v>
       </c>
     </row>
     <row r="1080">
@@ -65604,7 +65607,7 @@
         <v>4888</v>
       </c>
       <c r="D1088" s="51" t="s">
-        <v>6417</v>
+        <v>6418</v>
       </c>
     </row>
     <row r="1089">
@@ -65660,7 +65663,7 @@
         <v>4906</v>
       </c>
       <c r="D1092" s="51" t="s">
-        <v>6418</v>
+        <v>6419</v>
       </c>
     </row>
     <row r="1093">
@@ -66007,7 +66010,7 @@
         <v>5027</v>
       </c>
       <c r="C1117" s="27" t="s">
-        <v>6419</v>
+        <v>6420</v>
       </c>
       <c r="D1117" s="59" t="s">
         <v>5030</v>
@@ -66542,7 +66545,7 @@
         <v>5218</v>
       </c>
       <c r="D1155" s="51" t="s">
-        <v>6420</v>
+        <v>6421</v>
       </c>
     </row>
     <row r="1156">
@@ -66749,7 +66752,7 @@
         <v>5282</v>
       </c>
       <c r="C1170" s="27" t="s">
-        <v>6421</v>
+        <v>6422</v>
       </c>
       <c r="D1170" s="52" t="s">
         <v>5285</v>
@@ -67785,10 +67788,10 @@
         <v>5604</v>
       </c>
       <c r="C1244" s="27" t="s">
-        <v>6422</v>
+        <v>6423</v>
       </c>
       <c r="D1244" s="59" t="s">
-        <v>6423</v>
+        <v>6424</v>
       </c>
     </row>
     <row r="1245">

</xml_diff>

<commit_message>
Wallet Connect strings (#167)
* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

---------

Co-authored-by: touge <touge1027@gmail.com>
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_387E3E20_2502_4B36_92B3_684C852B578A_.wvu.FilterData">'client strings'!$D$1:$D$1481</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_5B9378D0_432D_4047_B219_D358CCFA3F9E_.wvu.FilterData">'client strings'!$C$1:$C$1481</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_89EC4390_DB7B_46E2_9AEA_D9B7AFD6A8C9_.wvu.FilterData">'client strings'!$D$1:$D$1481</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FAC47341_407B_4ED0_90AD_C05847F28EBF_.wvu.FilterData">'client strings'!$C$1:$C$1481</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{5B9378D0-432D-4047-B219-D358CCFA3F9E}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{387E3E20-2502-4B36-92B3-684C852B578A}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FAC47341-407B-4ED0-90AD-C05847F28EBF}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{89EC4390-DB7B-46E2-9AEA-D9B7AFD6A8C9}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14505" uniqueCount="6694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14637" uniqueCount="6790">
   <si>
     <t>platform</t>
   </si>
@@ -20058,6 +20058,294 @@
   </si>
   <si>
     <t>System</t>
+  </si>
+  <si>
+    <t>request_rejected</t>
+  </si>
+  <si>
+    <t>Request Rejected</t>
+  </si>
+  <si>
+    <t>请求已拒绝</t>
+  </si>
+  <si>
+    <t>request_rejected_reason_another_request_in_process</t>
+  </si>
+  <si>
+    <t>Another request is in process, please retry after current request is finished</t>
+  </si>
+  <si>
+    <t>正在处理另一请求，请完成当前请求后重试</t>
+  </si>
+  <si>
+    <t>connection_failed</t>
+  </si>
+  <si>
+    <t>Connection Failed</t>
+  </si>
+  <si>
+    <t>连接失败</t>
+  </si>
+  <si>
+    <t>chain_not_supported</t>
+  </si>
+  <si>
+    <t>Chain not supported</t>
+  </si>
+  <si>
+    <t>不支持此网络</t>
+  </si>
+  <si>
+    <t>session_not_found</t>
+  </si>
+  <si>
+    <t>Session not found</t>
+  </si>
+  <si>
+    <t>没有对应的连接</t>
+  </si>
+  <si>
+    <t>unable_to_decode_the_request</t>
+  </si>
+  <si>
+    <t>Unable to decode the request: %1$s</t>
+  </si>
+  <si>
+    <t>无法解析请求: %1$s</t>
+  </si>
+  <si>
+    <t>method_not_supported</t>
+  </si>
+  <si>
+    <t>Method %1$s is not supported</t>
+  </si>
+  <si>
+    <t>不支持此方法: %1$s</t>
+  </si>
+  <si>
+    <t>switch_network</t>
+  </si>
+  <si>
+    <t>Switch Network</t>
+  </si>
+  <si>
+    <t>切换网络</t>
+  </si>
+  <si>
+    <t>requests_switching_to_network</t>
+  </si>
+  <si>
+    <t>%1$s requests switching to %2$s</t>
+  </si>
+  <si>
+    <t>%1$s 请求切换到 %2$s</t>
+  </si>
+  <si>
+    <t>switch_to_network</t>
+  </si>
+  <si>
+    <t>Switch to %1$s</t>
+  </si>
+  <si>
+    <t>切换到 %1$s</t>
+  </si>
+  <si>
+    <t>keep_network</t>
+  </si>
+  <si>
+    <t>Keep %1$s</t>
+  </si>
+  <si>
+    <t>留在 %1$s</t>
+  </si>
+  <si>
+    <t>network_switched</t>
+  </si>
+  <si>
+    <t>Network Switched</t>
+  </si>
+  <si>
+    <t>已切换网络</t>
+  </si>
+  <si>
+    <t>failed_to_switch_network</t>
+  </si>
+  <si>
+    <t>Failed to switch network: %1$s</t>
+  </si>
+  <si>
+    <t>切换网络失败: %1$s</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>网络</t>
+  </si>
+  <si>
+    <t>connect_wallet</t>
+  </si>
+  <si>
+    <t>Connect Wallet</t>
+  </si>
+  <si>
+    <t>连接钱包</t>
+  </si>
+  <si>
+    <t>read_your_public_address</t>
+  </si>
+  <si>
+    <t>Read your public address</t>
+  </si>
+  <si>
+    <t>读取你的地址</t>
+  </si>
+  <si>
+    <t>allow_dapp_access_public_address</t>
+  </si>
+  <si>
+    <t>Allow app to access your wallet balance and activity.</t>
+  </si>
+  <si>
+    <t>允许App访问你的钱包余额及活动。</t>
+  </si>
+  <si>
+    <t>request_permission</t>
+  </si>
+  <si>
+    <t>Request permission</t>
+  </si>
+  <si>
+    <t>允许请求</t>
+  </si>
+  <si>
+    <t>allow_dapp_request_permission</t>
+  </si>
+  <si>
+    <t>Allow dapp to ask for your permission to make a transaction.</t>
+  </si>
+  <si>
+    <t>允许Dapp向你发送请求，如转账请求等</t>
+  </si>
+  <si>
+    <t>丢弃</t>
+  </si>
+  <si>
+    <t>send_signed_message_confirmation</t>
+  </si>
+  <si>
+    <t>The message has been signed successfully, click the button below to send or discard the signed message</t>
+  </si>
+  <si>
+    <t>此消息已被签名，点击下方按钮以发送或丢弃</t>
+  </si>
+  <si>
+    <t>signature_request</t>
+  </si>
+  <si>
+    <t>Signature Request</t>
+  </si>
+  <si>
+    <t>请求签名</t>
+  </si>
+  <si>
+    <t>transaction_request</t>
+  </si>
+  <si>
+    <t>Transaction Request</t>
+  </si>
+  <si>
+    <t>请求转账</t>
+  </si>
+  <si>
+    <t>calculating</t>
+  </si>
+  <si>
+    <t>Calculating…</t>
+  </si>
+  <si>
+    <t>正在计算…</t>
+  </si>
+  <si>
+    <t>transaction_failed</t>
+  </si>
+  <si>
+    <t>Transaction Failed</t>
+  </si>
+  <si>
+    <t>转账失败</t>
+  </si>
+  <si>
+    <t>Network Fee</t>
+  </si>
+  <si>
+    <t>网络费用</t>
+  </si>
+  <si>
+    <t>signature_request_warning</t>
+  </si>
+  <si>
+    <t>We cannot verify this signature request. Make sure you trust this app before signing this request.</t>
+  </si>
+  <si>
+    <t>我们无法验证此请求。签名前请确认你信任此App。</t>
+  </si>
+  <si>
+    <t>sign_by_pin</t>
+  </si>
+  <si>
+    <t>Sign by PIN</t>
+  </si>
+  <si>
+    <t>使用PIN签名</t>
+  </si>
+  <si>
+    <t>dapp_description</t>
+  </si>
+  <si>
+    <t>This dapp has connected to your wallet, it can view your wallet balance, activity and request approval for transactions.</t>
+  </si>
+  <si>
+    <t>此Dapp已经与你的钱包连接，并被授权查看你的钱包余额及活动，也可向你发出转账请求。</t>
+  </si>
+  <si>
+    <t>disconnected</t>
+  </si>
+  <si>
+    <t>Disconnected</t>
+  </si>
+  <si>
+    <t>已断开</t>
+  </si>
+  <si>
+    <t>no_dapp</t>
+  </si>
+  <si>
+    <t>No dapp</t>
+  </si>
+  <si>
+    <t>没有Dapp</t>
+  </si>
+  <si>
+    <t>connected_dapps</t>
+  </si>
+  <si>
+    <t>Connected Dapps</t>
+  </si>
+  <si>
+    <t>已连接的Dapp</t>
+  </si>
+  <si>
+    <t>search_placeholder_dapp</t>
+  </si>
+  <si>
+    <t>Name, URL</t>
+  </si>
+  <si>
+    <t>名称, URL</t>
   </si>
   <si>
     <t>AppStore</t>
@@ -52536,73 +52824,622 @@
     </row>
     <row r="1516" ht="15.75" customHeight="1">
       <c r="A1516" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1516" s="1"/>
-      <c r="C1516" s="1"/>
-      <c r="D1516" s="1"/>
+        <v>1305</v>
+      </c>
+      <c r="B1516" s="1" t="s">
+        <v>6659</v>
+      </c>
+      <c r="C1516" s="1" t="s">
+        <v>6660</v>
+      </c>
+      <c r="D1516" s="1" t="s">
+        <v>6661</v>
+      </c>
       <c r="E1516" s="13"/>
       <c r="F1516" s="4"/>
       <c r="G1516" s="4"/>
     </row>
-    <row r="1517" ht="15.75" customHeight="1">
+    <row r="1517">
       <c r="A1517" s="1" t="s">
-        <v>6659</v>
-      </c>
-      <c r="B1517" s="1"/>
+        <v>1305</v>
+      </c>
+      <c r="B1517" s="1" t="s">
+        <v>6662</v>
+      </c>
       <c r="C1517" s="1" t="s">
-        <v>6660</v>
-      </c>
-      <c r="D1517" s="1"/>
-      <c r="E1517" s="13"/>
-      <c r="F1517" s="4"/>
-      <c r="G1517" s="4"/>
-    </row>
-    <row r="1518" ht="15.75" customHeight="1">
+        <v>6663</v>
+      </c>
+      <c r="D1517" s="1" t="s">
+        <v>6664</v>
+      </c>
+    </row>
+    <row r="1518">
       <c r="A1518" s="1" t="s">
-        <v>6659</v>
-      </c>
-      <c r="B1518" s="1"/>
+        <v>1305</v>
+      </c>
+      <c r="B1518" s="1" t="s">
+        <v>6665</v>
+      </c>
       <c r="C1518" s="1" t="s">
-        <v>6661</v>
-      </c>
-      <c r="D1518" s="1"/>
-      <c r="E1518" s="13"/>
-      <c r="F1518" s="4"/>
-      <c r="G1518" s="4"/>
-    </row>
-    <row r="1519" ht="15.75" customHeight="1">
+        <v>6666</v>
+      </c>
+      <c r="D1518" s="1" t="s">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="1519">
       <c r="A1519" s="1" t="s">
-        <v>6659</v>
-      </c>
-      <c r="B1519" s="1"/>
+        <v>1305</v>
+      </c>
+      <c r="B1519" s="1" t="s">
+        <v>6668</v>
+      </c>
       <c r="C1519" s="1" t="s">
-        <v>6662</v>
-      </c>
-      <c r="D1519" s="1"/>
-      <c r="E1519" s="13"/>
-      <c r="F1519" s="4"/>
-      <c r="G1519" s="4"/>
-    </row>
-    <row r="1520" ht="15.75" customHeight="1">
+        <v>6669</v>
+      </c>
+      <c r="D1519" s="1" t="s">
+        <v>6670</v>
+      </c>
+    </row>
+    <row r="1520">
       <c r="A1520" s="1" t="s">
-        <v>6659</v>
-      </c>
-      <c r="B1520" s="1"/>
+        <v>1305</v>
+      </c>
+      <c r="B1520" s="1" t="s">
+        <v>6671</v>
+      </c>
       <c r="C1520" s="1" t="s">
-        <v>6663</v>
-      </c>
-      <c r="D1520" s="1"/>
-      <c r="E1520" s="13"/>
-      <c r="F1520" s="4"/>
-      <c r="G1520" s="4"/>
+        <v>6672</v>
+      </c>
+      <c r="D1520" s="1" t="s">
+        <v>6673</v>
+      </c>
+    </row>
+    <row r="1521" ht="15.75" customHeight="1">
+      <c r="A1521" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1521" s="1" t="s">
+        <v>6674</v>
+      </c>
+      <c r="C1521" s="1" t="s">
+        <v>6675</v>
+      </c>
+      <c r="D1521" s="1" t="s">
+        <v>6676</v>
+      </c>
+      <c r="E1521" s="13"/>
+      <c r="F1521" s="4"/>
+      <c r="G1521" s="4"/>
+    </row>
+    <row r="1522" ht="15.75" customHeight="1">
+      <c r="A1522" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1522" s="1" t="s">
+        <v>6677</v>
+      </c>
+      <c r="C1522" s="1" t="s">
+        <v>6678</v>
+      </c>
+      <c r="D1522" s="1" t="s">
+        <v>6679</v>
+      </c>
+      <c r="E1522" s="13"/>
+      <c r="F1522" s="4"/>
+      <c r="G1522" s="4"/>
+    </row>
+    <row r="1523" ht="15.75" customHeight="1">
+      <c r="A1523" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1523" s="1" t="s">
+        <v>6680</v>
+      </c>
+      <c r="C1523" s="1" t="s">
+        <v>6681</v>
+      </c>
+      <c r="D1523" s="1" t="s">
+        <v>6682</v>
+      </c>
+      <c r="E1523" s="13"/>
+      <c r="F1523" s="4"/>
+      <c r="G1523" s="4"/>
+    </row>
+    <row r="1524" ht="15.75" customHeight="1">
+      <c r="A1524" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1524" s="1" t="s">
+        <v>6683</v>
+      </c>
+      <c r="C1524" s="1" t="s">
+        <v>6684</v>
+      </c>
+      <c r="D1524" s="1" t="s">
+        <v>6685</v>
+      </c>
+      <c r="E1524" s="13"/>
+      <c r="F1524" s="4"/>
+      <c r="G1524" s="4"/>
+    </row>
+    <row r="1525" ht="15.75" customHeight="1">
+      <c r="A1525" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1525" s="1" t="s">
+        <v>6686</v>
+      </c>
+      <c r="C1525" s="1" t="s">
+        <v>6687</v>
+      </c>
+      <c r="D1525" s="1" t="s">
+        <v>6688</v>
+      </c>
+      <c r="E1525" s="13"/>
+      <c r="F1525" s="4"/>
+      <c r="G1525" s="4"/>
+    </row>
+    <row r="1526" ht="15.75" customHeight="1">
+      <c r="A1526" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1526" s="1" t="s">
+        <v>6689</v>
+      </c>
+      <c r="C1526" s="1" t="s">
+        <v>6690</v>
+      </c>
+      <c r="D1526" s="1" t="s">
+        <v>6691</v>
+      </c>
+      <c r="E1526" s="13"/>
+      <c r="F1526" s="4"/>
+      <c r="G1526" s="4"/>
+    </row>
+    <row r="1527" ht="15.75" customHeight="1">
+      <c r="A1527" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1527" s="1" t="s">
+        <v>6692</v>
+      </c>
+      <c r="C1527" s="1" t="s">
+        <v>6693</v>
+      </c>
+      <c r="D1527" s="1" t="s">
+        <v>6694</v>
+      </c>
+      <c r="E1527" s="13"/>
+      <c r="F1527" s="4"/>
+      <c r="G1527" s="4"/>
+    </row>
+    <row r="1528" ht="15.75" customHeight="1">
+      <c r="A1528" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1528" s="1" t="s">
+        <v>6695</v>
+      </c>
+      <c r="C1528" s="1" t="s">
+        <v>6696</v>
+      </c>
+      <c r="D1528" s="1" t="s">
+        <v>6697</v>
+      </c>
+      <c r="E1528" s="13"/>
+      <c r="F1528" s="4"/>
+      <c r="G1528" s="4"/>
+    </row>
+    <row r="1529" ht="15.75" customHeight="1">
+      <c r="A1529" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1529" s="1" t="s">
+        <v>6698</v>
+      </c>
+      <c r="C1529" s="1" t="s">
+        <v>6699</v>
+      </c>
+      <c r="D1529" s="1" t="s">
+        <v>6700</v>
+      </c>
+      <c r="E1529" s="13"/>
+      <c r="F1529" s="4"/>
+      <c r="G1529" s="4"/>
+    </row>
+    <row r="1530" ht="15.75" customHeight="1">
+      <c r="A1530" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1530" s="1" t="s">
+        <v>6701</v>
+      </c>
+      <c r="C1530" s="1" t="s">
+        <v>6702</v>
+      </c>
+      <c r="D1530" s="1" t="s">
+        <v>6703</v>
+      </c>
+      <c r="E1530" s="13"/>
+      <c r="F1530" s="4"/>
+      <c r="G1530" s="4"/>
+    </row>
+    <row r="1531" ht="15.75" customHeight="1">
+      <c r="A1531" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1531" s="1" t="s">
+        <v>6704</v>
+      </c>
+      <c r="C1531" s="1" t="s">
+        <v>6705</v>
+      </c>
+      <c r="D1531" s="1" t="s">
+        <v>6706</v>
+      </c>
+      <c r="E1531" s="13"/>
+      <c r="F1531" s="4"/>
+      <c r="G1531" s="4"/>
+    </row>
+    <row r="1532" ht="15.75" customHeight="1">
+      <c r="A1532" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1532" s="1" t="s">
+        <v>6707</v>
+      </c>
+      <c r="C1532" s="1" t="s">
+        <v>6708</v>
+      </c>
+      <c r="D1532" s="1" t="s">
+        <v>6709</v>
+      </c>
+      <c r="E1532" s="13"/>
+      <c r="F1532" s="4"/>
+      <c r="G1532" s="4"/>
+    </row>
+    <row r="1533" ht="15.75" customHeight="1">
+      <c r="A1533" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1533" s="1" t="s">
+        <v>6710</v>
+      </c>
+      <c r="C1533" s="1" t="s">
+        <v>6711</v>
+      </c>
+      <c r="D1533" s="1" t="s">
+        <v>6712</v>
+      </c>
+      <c r="E1533" s="13"/>
+      <c r="F1533" s="4"/>
+      <c r="G1533" s="4"/>
+    </row>
+    <row r="1534" ht="15.75" customHeight="1">
+      <c r="A1534" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1534" s="1" t="s">
+        <v>6713</v>
+      </c>
+      <c r="C1534" s="1" t="s">
+        <v>6714</v>
+      </c>
+      <c r="D1534" s="1" t="s">
+        <v>6715</v>
+      </c>
+      <c r="E1534" s="13"/>
+      <c r="F1534" s="4"/>
+      <c r="G1534" s="4"/>
+    </row>
+    <row r="1535" ht="15.75" customHeight="1">
+      <c r="A1535" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1535" s="1" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C1535" s="1" t="s">
+        <v>2128</v>
+      </c>
+      <c r="D1535" s="1" t="s">
+        <v>6716</v>
+      </c>
+      <c r="E1535" s="13"/>
+      <c r="F1535" s="4"/>
+      <c r="G1535" s="4"/>
+    </row>
+    <row r="1536" ht="15.75" customHeight="1">
+      <c r="A1536" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1536" s="1" t="s">
+        <v>6717</v>
+      </c>
+      <c r="C1536" s="1" t="s">
+        <v>6718</v>
+      </c>
+      <c r="D1536" s="1" t="s">
+        <v>6719</v>
+      </c>
+      <c r="E1536" s="13"/>
+      <c r="F1536" s="4"/>
+      <c r="G1536" s="4"/>
+    </row>
+    <row r="1537" ht="15.75" customHeight="1">
+      <c r="A1537" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1537" s="1" t="s">
+        <v>6720</v>
+      </c>
+      <c r="C1537" s="1" t="s">
+        <v>6721</v>
+      </c>
+      <c r="D1537" s="1" t="s">
+        <v>6722</v>
+      </c>
+      <c r="E1537" s="13"/>
+      <c r="F1537" s="4"/>
+      <c r="G1537" s="4"/>
+    </row>
+    <row r="1538" ht="15.75" customHeight="1">
+      <c r="A1538" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1538" s="1" t="s">
+        <v>6723</v>
+      </c>
+      <c r="C1538" s="1" t="s">
+        <v>6724</v>
+      </c>
+      <c r="D1538" s="1" t="s">
+        <v>6725</v>
+      </c>
+      <c r="E1538" s="13"/>
+      <c r="F1538" s="4"/>
+      <c r="G1538" s="4"/>
+    </row>
+    <row r="1539" ht="15.75" customHeight="1">
+      <c r="A1539" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1539" s="1" t="s">
+        <v>6726</v>
+      </c>
+      <c r="C1539" s="1" t="s">
+        <v>6727</v>
+      </c>
+      <c r="D1539" s="1" t="s">
+        <v>6728</v>
+      </c>
+      <c r="E1539" s="13"/>
+      <c r="F1539" s="4"/>
+      <c r="G1539" s="4"/>
+    </row>
+    <row r="1540" ht="15.75" customHeight="1">
+      <c r="A1540" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1540" s="1" t="s">
+        <v>6729</v>
+      </c>
+      <c r="C1540" s="1" t="s">
+        <v>6730</v>
+      </c>
+      <c r="D1540" s="1" t="s">
+        <v>6731</v>
+      </c>
+      <c r="E1540" s="13"/>
+      <c r="F1540" s="4"/>
+      <c r="G1540" s="4"/>
+    </row>
+    <row r="1541" ht="15.75" customHeight="1">
+      <c r="A1541" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1541" s="1" t="s">
+        <v>3740</v>
+      </c>
+      <c r="C1541" s="1" t="s">
+        <v>6732</v>
+      </c>
+      <c r="D1541" s="1" t="s">
+        <v>6733</v>
+      </c>
+      <c r="E1541" s="13"/>
+      <c r="F1541" s="4"/>
+      <c r="G1541" s="4"/>
+    </row>
+    <row r="1542" ht="15.75" customHeight="1">
+      <c r="A1542" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1542" s="1" t="s">
+        <v>6734</v>
+      </c>
+      <c r="C1542" s="1" t="s">
+        <v>6735</v>
+      </c>
+      <c r="D1542" s="1" t="s">
+        <v>6736</v>
+      </c>
+      <c r="E1542" s="13"/>
+      <c r="F1542" s="4"/>
+      <c r="G1542" s="4"/>
+    </row>
+    <row r="1543" ht="15.75" customHeight="1">
+      <c r="A1543" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1543" s="1" t="s">
+        <v>6737</v>
+      </c>
+      <c r="C1543" s="1" t="s">
+        <v>6738</v>
+      </c>
+      <c r="D1543" s="1" t="s">
+        <v>6739</v>
+      </c>
+      <c r="E1543" s="13"/>
+      <c r="F1543" s="4"/>
+      <c r="G1543" s="4"/>
+    </row>
+    <row r="1544" ht="15.75" customHeight="1">
+      <c r="A1544" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1544" s="1" t="s">
+        <v>6740</v>
+      </c>
+      <c r="C1544" s="1" t="s">
+        <v>6741</v>
+      </c>
+      <c r="D1544" s="1" t="s">
+        <v>6742</v>
+      </c>
+      <c r="E1544" s="13"/>
+      <c r="F1544" s="4"/>
+      <c r="G1544" s="4"/>
+    </row>
+    <row r="1545" ht="15.75" customHeight="1">
+      <c r="A1545" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1545" s="1" t="s">
+        <v>6743</v>
+      </c>
+      <c r="C1545" s="1" t="s">
+        <v>6744</v>
+      </c>
+      <c r="D1545" s="1" t="s">
+        <v>6745</v>
+      </c>
+      <c r="E1545" s="13"/>
+      <c r="F1545" s="4"/>
+      <c r="G1545" s="4"/>
+    </row>
+    <row r="1546" ht="15.75" customHeight="1">
+      <c r="A1546" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1546" s="1" t="s">
+        <v>6746</v>
+      </c>
+      <c r="C1546" s="1" t="s">
+        <v>6747</v>
+      </c>
+      <c r="D1546" s="1" t="s">
+        <v>6748</v>
+      </c>
+      <c r="E1546" s="13"/>
+      <c r="F1546" s="4"/>
+      <c r="G1546" s="4"/>
+    </row>
+    <row r="1547" ht="15.75" customHeight="1">
+      <c r="A1547" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1547" s="1" t="s">
+        <v>6749</v>
+      </c>
+      <c r="C1547" s="1" t="s">
+        <v>6750</v>
+      </c>
+      <c r="D1547" s="1" t="s">
+        <v>6751</v>
+      </c>
+      <c r="E1547" s="13"/>
+      <c r="F1547" s="4"/>
+      <c r="G1547" s="4"/>
+    </row>
+    <row r="1548" ht="15.75" customHeight="1">
+      <c r="A1548" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1548" s="1" t="s">
+        <v>6752</v>
+      </c>
+      <c r="C1548" s="1" t="s">
+        <v>6753</v>
+      </c>
+      <c r="D1548" s="1" t="s">
+        <v>6754</v>
+      </c>
+      <c r="E1548" s="13"/>
+      <c r="F1548" s="4"/>
+      <c r="G1548" s="4"/>
+    </row>
+    <row r="1549" ht="15.75" customHeight="1">
+      <c r="A1549" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1549" s="1"/>
+      <c r="C1549" s="1"/>
+      <c r="D1549" s="1"/>
+      <c r="E1549" s="13"/>
+      <c r="F1549" s="4"/>
+      <c r="G1549" s="4"/>
+    </row>
+    <row r="1550" ht="15.75" customHeight="1">
+      <c r="A1550" s="1" t="s">
+        <v>6755</v>
+      </c>
+      <c r="B1550" s="1"/>
+      <c r="C1550" s="1" t="s">
+        <v>6756</v>
+      </c>
+      <c r="D1550" s="1"/>
+      <c r="E1550" s="13"/>
+      <c r="F1550" s="4"/>
+      <c r="G1550" s="4"/>
+    </row>
+    <row r="1551" ht="15.75" customHeight="1">
+      <c r="A1551" s="1" t="s">
+        <v>6755</v>
+      </c>
+      <c r="B1551" s="1"/>
+      <c r="C1551" s="1" t="s">
+        <v>6757</v>
+      </c>
+      <c r="D1551" s="1"/>
+      <c r="E1551" s="13"/>
+      <c r="F1551" s="4"/>
+      <c r="G1551" s="4"/>
+    </row>
+    <row r="1552" ht="15.75" customHeight="1">
+      <c r="A1552" s="1" t="s">
+        <v>6755</v>
+      </c>
+      <c r="B1552" s="1"/>
+      <c r="C1552" s="1" t="s">
+        <v>6758</v>
+      </c>
+      <c r="D1552" s="1"/>
+      <c r="E1552" s="13"/>
+      <c r="F1552" s="4"/>
+      <c r="G1552" s="4"/>
+    </row>
+    <row r="1553" ht="15.75" customHeight="1">
+      <c r="A1553" s="1" t="s">
+        <v>6755</v>
+      </c>
+      <c r="B1553" s="1"/>
+      <c r="C1553" s="1" t="s">
+        <v>6759</v>
+      </c>
+      <c r="D1553" s="1"/>
+      <c r="E1553" s="13"/>
+      <c r="F1553" s="4"/>
+      <c r="G1553" s="4"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{387E3E20-2502-4B36-92B3-684C852B578A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{89EC4390-DB7B-46E2-9AEA-D9B7AFD6A8C9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1481"/>
     </customSheetView>
-    <customSheetView guid="{5B9378D0-432D-4047-B219-D358CCFA3F9E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FAC47341-407B-4ED0-90AD-C05847F28EBF}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1481"/>
     </customSheetView>
   </customSheetViews>
@@ -52613,17 +53450,17 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B206:B207">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>COUNTIF(C206:C1638, B206) &gt; 1</formula>
+      <formula>COUNTIF(C206:C1671, B206) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B166:B193">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COUNTIF(C166:C1617, B166) &gt; 1</formula>
+      <formula>COUNTIF(C166:C1650, B166) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B195:B205">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>COUNTIF(C195:C1618, B195) &gt; 1</formula>
+      <formula>COUNTIF(C195:C1651, B195) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -55490,7 +56327,7 @@
         <v>1016</v>
       </c>
       <c r="C202" s="28" t="s">
-        <v>6664</v>
+        <v>6760</v>
       </c>
       <c r="D202" s="69" t="s">
         <v>1019</v>
@@ -56383,10 +57220,10 @@
         <v>7</v>
       </c>
       <c r="B266" s="28" t="s">
-        <v>6665</v>
+        <v>6761</v>
       </c>
       <c r="C266" s="28" t="s">
-        <v>6665</v>
+        <v>6761</v>
       </c>
       <c r="D266" s="54" t="s">
         <v>746</v>
@@ -56974,7 +57811,7 @@
         <v>1517</v>
       </c>
       <c r="C308" s="74" t="s">
-        <v>6666</v>
+        <v>6762</v>
       </c>
       <c r="D308" s="53" t="s">
         <v>1520</v>
@@ -62073,7 +62910,7 @@
         <v>3224</v>
       </c>
       <c r="D672" s="87" t="s">
-        <v>6667</v>
+        <v>6763</v>
       </c>
     </row>
     <row r="673">
@@ -62725,13 +63562,13 @@
         <v>139</v>
       </c>
       <c r="B719" s="28" t="s">
-        <v>6668</v>
+        <v>6764</v>
       </c>
       <c r="C719" s="27" t="s">
-        <v>6669</v>
+        <v>6765</v>
       </c>
       <c r="D719" s="82" t="s">
-        <v>6670</v>
+        <v>6766</v>
       </c>
     </row>
     <row r="720">
@@ -64223,10 +65060,10 @@
         <v>139</v>
       </c>
       <c r="B826" s="28" t="s">
-        <v>6671</v>
+        <v>6767</v>
       </c>
       <c r="C826" s="28" t="s">
-        <v>6672</v>
+        <v>6768</v>
       </c>
       <c r="D826" s="53" t="s">
         <v>3935</v>
@@ -66175,7 +67012,7 @@
         <v>4588</v>
       </c>
       <c r="D965" s="53" t="s">
-        <v>6673</v>
+        <v>6769</v>
       </c>
     </row>
     <row r="966">
@@ -67561,7 +68398,7 @@
         <v>5043</v>
       </c>
       <c r="D1064" s="53" t="s">
-        <v>6674</v>
+        <v>6770</v>
       </c>
     </row>
     <row r="1065">
@@ -67589,7 +68426,7 @@
         <v>5051</v>
       </c>
       <c r="D1066" s="53" t="s">
-        <v>6675</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="1067">
@@ -67617,7 +68454,7 @@
         <v>5059</v>
       </c>
       <c r="D1068" s="53" t="s">
-        <v>6676</v>
+        <v>6772</v>
       </c>
     </row>
     <row r="1069">
@@ -67659,7 +68496,7 @@
         <v>5074</v>
       </c>
       <c r="D1071" s="54" t="s">
-        <v>6677</v>
+        <v>6773</v>
       </c>
     </row>
     <row r="1072">
@@ -67729,7 +68566,7 @@
         <v>5090</v>
       </c>
       <c r="D1076" s="63" t="s">
-        <v>6678</v>
+        <v>6774</v>
       </c>
     </row>
     <row r="1077">
@@ -67771,7 +68608,7 @@
         <v>5104</v>
       </c>
       <c r="D1079" s="53" t="s">
-        <v>6679</v>
+        <v>6775</v>
       </c>
     </row>
     <row r="1080">
@@ -67897,7 +68734,7 @@
         <v>5145</v>
       </c>
       <c r="D1088" s="53" t="s">
-        <v>6680</v>
+        <v>6776</v>
       </c>
     </row>
     <row r="1089">
@@ -67953,7 +68790,7 @@
         <v>5163</v>
       </c>
       <c r="D1092" s="53" t="s">
-        <v>6681</v>
+        <v>6777</v>
       </c>
     </row>
     <row r="1093">
@@ -68300,7 +69137,7 @@
         <v>5290</v>
       </c>
       <c r="C1117" s="28" t="s">
-        <v>6682</v>
+        <v>6778</v>
       </c>
       <c r="D1117" s="61" t="s">
         <v>5293</v>
@@ -68835,7 +69672,7 @@
         <v>5481</v>
       </c>
       <c r="D1155" s="53" t="s">
-        <v>6683</v>
+        <v>6779</v>
       </c>
     </row>
     <row r="1156">
@@ -69042,7 +69879,7 @@
         <v>5545</v>
       </c>
       <c r="C1170" s="28" t="s">
-        <v>6684</v>
+        <v>6780</v>
       </c>
       <c r="D1170" s="54" t="s">
         <v>5548</v>
@@ -70078,10 +70915,10 @@
         <v>5889</v>
       </c>
       <c r="C1244" s="28" t="s">
-        <v>6685</v>
+        <v>6781</v>
       </c>
       <c r="D1244" s="61" t="s">
-        <v>6686</v>
+        <v>6782</v>
       </c>
     </row>
     <row r="1245">
@@ -71405,13 +72242,13 @@
         <v>84</v>
       </c>
       <c r="B1339" s="28" t="s">
-        <v>6687</v>
+        <v>6783</v>
       </c>
       <c r="C1339" s="27" t="s">
-        <v>6688</v>
+        <v>6784</v>
       </c>
       <c r="D1339" s="59" t="s">
-        <v>6689</v>
+        <v>6785</v>
       </c>
     </row>
     <row r="1340">
@@ -71590,7 +72427,7 @@
         <v>6391</v>
       </c>
       <c r="C1352" s="27" t="s">
-        <v>6690</v>
+        <v>6786</v>
       </c>
       <c r="D1352" s="81" t="s">
         <v>6394</v>
@@ -72203,13 +73040,13 @@
         <v>53</v>
       </c>
       <c r="B1396" s="28" t="s">
-        <v>6691</v>
+        <v>6787</v>
       </c>
       <c r="C1396" s="27" t="s">
-        <v>6692</v>
+        <v>6788</v>
       </c>
       <c r="D1396" s="59" t="s">
-        <v>6693</v>
+        <v>6789</v>
       </c>
     </row>
     <row r="1397">

</xml_diff>

<commit_message>
Remove a duplicated string (#169)
* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs

---------

Co-authored-by: touge <touge1027@gmail.com>
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_6AB487A3_A910_4D20_927D_20206084AAC6_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_E2C8D0AD_A6EE_4C7B_B202_9DADB2D411EA_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DC9169F3_CEC1_48DA_9009_37A06AC1058B_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_2B9E84B6_F9B5_4F00_9170_DF49C5FE68A3_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E2C8D0AD-A6EE-4C7B-B202-9DADB2D411EA}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6AB487A3-A910-4D20-927D-20206084AAC6}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2B9E84B6-F9B5-4F00-9170-DF49C5FE68A3}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC9169F3-CEC1-48DA-9009-37A06AC1058B}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14631" uniqueCount="6789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14627" uniqueCount="6788">
   <si>
     <t>platform</t>
   </si>
@@ -20217,9 +20217,6 @@
   </si>
   <si>
     <t>允许 Dapp 向你发送请求，如转账请求等</t>
-  </si>
-  <si>
-    <t>丢弃</t>
   </si>
   <si>
     <t>send_signed_message_confirmation</t>
@@ -31369,7 +31366,7 @@
     </row>
     <row r="490" ht="15.75" customHeight="1">
       <c r="A490" s="1" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="B490" s="1" t="s">
         <v>2127</v>
@@ -53116,13 +53113,13 @@
         <v>1305</v>
       </c>
       <c r="B1534" s="1" t="s">
-        <v>2127</v>
+        <v>6712</v>
       </c>
       <c r="C1534" s="1" t="s">
-        <v>2128</v>
+        <v>6713</v>
       </c>
       <c r="D1534" s="1" t="s">
-        <v>6712</v>
+        <v>6714</v>
       </c>
       <c r="E1534" s="13"/>
       <c r="F1534" s="4"/>
@@ -53133,13 +53130,13 @@
         <v>1305</v>
       </c>
       <c r="B1535" s="1" t="s">
-        <v>6713</v>
+        <v>6715</v>
       </c>
       <c r="C1535" s="1" t="s">
-        <v>6714</v>
+        <v>6716</v>
       </c>
       <c r="D1535" s="1" t="s">
-        <v>6715</v>
+        <v>6717</v>
       </c>
       <c r="E1535" s="13"/>
       <c r="F1535" s="4"/>
@@ -53150,13 +53147,13 @@
         <v>1305</v>
       </c>
       <c r="B1536" s="1" t="s">
-        <v>6716</v>
+        <v>6718</v>
       </c>
       <c r="C1536" s="1" t="s">
-        <v>6717</v>
+        <v>6719</v>
       </c>
       <c r="D1536" s="1" t="s">
-        <v>6718</v>
+        <v>6720</v>
       </c>
       <c r="E1536" s="13"/>
       <c r="F1536" s="4"/>
@@ -53167,13 +53164,13 @@
         <v>1305</v>
       </c>
       <c r="B1537" s="1" t="s">
-        <v>6719</v>
+        <v>6721</v>
       </c>
       <c r="C1537" s="1" t="s">
-        <v>6720</v>
+        <v>6722</v>
       </c>
       <c r="D1537" s="1" t="s">
-        <v>6721</v>
+        <v>6723</v>
       </c>
       <c r="E1537" s="13"/>
       <c r="F1537" s="4"/>
@@ -53184,13 +53181,13 @@
         <v>1305</v>
       </c>
       <c r="B1538" s="1" t="s">
-        <v>6722</v>
+        <v>6724</v>
       </c>
       <c r="C1538" s="1" t="s">
-        <v>6723</v>
+        <v>6725</v>
       </c>
       <c r="D1538" s="1" t="s">
-        <v>6724</v>
+        <v>6726</v>
       </c>
       <c r="E1538" s="13"/>
       <c r="F1538" s="4"/>
@@ -53201,13 +53198,13 @@
         <v>1305</v>
       </c>
       <c r="B1539" s="1" t="s">
-        <v>6725</v>
+        <v>6727</v>
       </c>
       <c r="C1539" s="1" t="s">
-        <v>6726</v>
+        <v>6728</v>
       </c>
       <c r="D1539" s="1" t="s">
-        <v>6727</v>
+        <v>6729</v>
       </c>
       <c r="E1539" s="13"/>
       <c r="F1539" s="4"/>
@@ -53218,13 +53215,13 @@
         <v>1305</v>
       </c>
       <c r="B1540" s="1" t="s">
-        <v>6728</v>
+        <v>6730</v>
       </c>
       <c r="C1540" s="1" t="s">
-        <v>6729</v>
+        <v>6731</v>
       </c>
       <c r="D1540" s="1" t="s">
-        <v>6730</v>
+        <v>6732</v>
       </c>
       <c r="E1540" s="13"/>
       <c r="F1540" s="4"/>
@@ -53235,13 +53232,13 @@
         <v>1305</v>
       </c>
       <c r="B1541" s="1" t="s">
-        <v>6731</v>
+        <v>6733</v>
       </c>
       <c r="C1541" s="1" t="s">
-        <v>6732</v>
+        <v>6734</v>
       </c>
       <c r="D1541" s="1" t="s">
-        <v>6733</v>
+        <v>6735</v>
       </c>
       <c r="E1541" s="13"/>
       <c r="F1541" s="4"/>
@@ -53252,13 +53249,13 @@
         <v>1305</v>
       </c>
       <c r="B1542" s="1" t="s">
-        <v>6734</v>
+        <v>6736</v>
       </c>
       <c r="C1542" s="1" t="s">
-        <v>6735</v>
+        <v>6737</v>
       </c>
       <c r="D1542" s="1" t="s">
-        <v>6736</v>
+        <v>6738</v>
       </c>
       <c r="E1542" s="13"/>
       <c r="F1542" s="4"/>
@@ -53269,13 +53266,13 @@
         <v>1305</v>
       </c>
       <c r="B1543" s="1" t="s">
-        <v>6737</v>
+        <v>6739</v>
       </c>
       <c r="C1543" s="1" t="s">
-        <v>6738</v>
+        <v>6740</v>
       </c>
       <c r="D1543" s="1" t="s">
-        <v>6739</v>
+        <v>6741</v>
       </c>
       <c r="E1543" s="13"/>
       <c r="F1543" s="4"/>
@@ -53286,13 +53283,13 @@
         <v>1305</v>
       </c>
       <c r="B1544" s="1" t="s">
-        <v>6740</v>
+        <v>6742</v>
       </c>
       <c r="C1544" s="1" t="s">
-        <v>6741</v>
+        <v>6743</v>
       </c>
       <c r="D1544" s="1" t="s">
-        <v>6742</v>
+        <v>6744</v>
       </c>
       <c r="E1544" s="13"/>
       <c r="F1544" s="4"/>
@@ -53303,13 +53300,13 @@
         <v>1305</v>
       </c>
       <c r="B1545" s="1" t="s">
-        <v>6743</v>
+        <v>6745</v>
       </c>
       <c r="C1545" s="1" t="s">
-        <v>6744</v>
+        <v>6746</v>
       </c>
       <c r="D1545" s="1" t="s">
-        <v>6745</v>
+        <v>6747</v>
       </c>
       <c r="E1545" s="13"/>
       <c r="F1545" s="4"/>
@@ -53320,13 +53317,13 @@
         <v>1305</v>
       </c>
       <c r="B1546" s="1" t="s">
-        <v>6746</v>
+        <v>6748</v>
       </c>
       <c r="C1546" s="1" t="s">
-        <v>6747</v>
+        <v>6749</v>
       </c>
       <c r="D1546" s="1" t="s">
-        <v>6748</v>
+        <v>6750</v>
       </c>
       <c r="E1546" s="13"/>
       <c r="F1546" s="4"/>
@@ -53334,24 +53331,20 @@
     </row>
     <row r="1547" ht="15.75" customHeight="1">
       <c r="A1547" s="1" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B1547" s="1" t="s">
-        <v>6749</v>
-      </c>
+        <v>6751</v>
+      </c>
+      <c r="B1547" s="1"/>
       <c r="C1547" s="1" t="s">
-        <v>6750</v>
-      </c>
-      <c r="D1547" s="1" t="s">
-        <v>6751</v>
-      </c>
+        <v>6752</v>
+      </c>
+      <c r="D1547" s="1"/>
       <c r="E1547" s="13"/>
       <c r="F1547" s="4"/>
       <c r="G1547" s="4"/>
     </row>
     <row r="1548" ht="15.75" customHeight="1">
       <c r="A1548" s="1" t="s">
-        <v>6752</v>
+        <v>6751</v>
       </c>
       <c r="B1548" s="1"/>
       <c r="C1548" s="1" t="s">
@@ -53364,7 +53357,7 @@
     </row>
     <row r="1549" ht="15.75" customHeight="1">
       <c r="A1549" s="1" t="s">
-        <v>6752</v>
+        <v>6751</v>
       </c>
       <c r="B1549" s="1"/>
       <c r="C1549" s="1" t="s">
@@ -53377,7 +53370,7 @@
     </row>
     <row r="1550" ht="15.75" customHeight="1">
       <c r="A1550" s="1" t="s">
-        <v>6752</v>
+        <v>6751</v>
       </c>
       <c r="B1550" s="1"/>
       <c r="C1550" s="1" t="s">
@@ -53388,25 +53381,12 @@
       <c r="F1550" s="4"/>
       <c r="G1550" s="4"/>
     </row>
-    <row r="1551" ht="15.75" customHeight="1">
-      <c r="A1551" s="1" t="s">
-        <v>6752</v>
-      </c>
-      <c r="B1551" s="1"/>
-      <c r="C1551" s="1" t="s">
-        <v>6756</v>
-      </c>
-      <c r="D1551" s="1"/>
-      <c r="E1551" s="13"/>
-      <c r="F1551" s="4"/>
-      <c r="G1551" s="4"/>
-    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6AB487A3-A910-4D20-927D-20206084AAC6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DC9169F3-CEC1-48DA-9009-37A06AC1058B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1480"/>
     </customSheetView>
-    <customSheetView guid="{E2C8D0AD-A6EE-4C7B-B202-9DADB2D411EA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2B9E84B6-F9B5-4F00-9170-DF49C5FE68A3}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1480"/>
     </customSheetView>
   </customSheetViews>
@@ -53417,17 +53397,17 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B206:B207">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>COUNTIF(C206:C1669, B206) &gt; 1</formula>
+      <formula>COUNTIF(C206:C1668, B206) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B166:B193">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>COUNTIF(C166:C1648, B166) &gt; 1</formula>
+      <formula>COUNTIF(C166:C1647, B166) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B195:B205">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>COUNTIF(C195:C1649, B195) &gt; 1</formula>
+      <formula>COUNTIF(C195:C1648, B195) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -56294,7 +56274,7 @@
         <v>1016</v>
       </c>
       <c r="C202" s="28" t="s">
-        <v>6757</v>
+        <v>6756</v>
       </c>
       <c r="D202" s="69" t="s">
         <v>1019</v>
@@ -57187,10 +57167,10 @@
         <v>7</v>
       </c>
       <c r="B266" s="28" t="s">
-        <v>6758</v>
+        <v>6757</v>
       </c>
       <c r="C266" s="28" t="s">
-        <v>6758</v>
+        <v>6757</v>
       </c>
       <c r="D266" s="54" t="s">
         <v>746</v>
@@ -57778,7 +57758,7 @@
         <v>1517</v>
       </c>
       <c r="C308" s="74" t="s">
-        <v>6759</v>
+        <v>6758</v>
       </c>
       <c r="D308" s="53" t="s">
         <v>1520</v>
@@ -62877,7 +62857,7 @@
         <v>3224</v>
       </c>
       <c r="D672" s="87" t="s">
-        <v>6760</v>
+        <v>6759</v>
       </c>
     </row>
     <row r="673">
@@ -63529,13 +63509,13 @@
         <v>139</v>
       </c>
       <c r="B719" s="28" t="s">
+        <v>6760</v>
+      </c>
+      <c r="C719" s="27" t="s">
         <v>6761</v>
       </c>
-      <c r="C719" s="27" t="s">
+      <c r="D719" s="82" t="s">
         <v>6762</v>
-      </c>
-      <c r="D719" s="82" t="s">
-        <v>6763</v>
       </c>
     </row>
     <row r="720">
@@ -64495,13 +64475,13 @@
         <v>68</v>
       </c>
       <c r="B788" s="28" t="s">
-        <v>6728</v>
+        <v>6727</v>
       </c>
       <c r="C788" s="28" t="s">
+        <v>6763</v>
+      </c>
+      <c r="D788" s="55" t="s">
         <v>6764</v>
-      </c>
-      <c r="D788" s="55" t="s">
-        <v>6765</v>
       </c>
     </row>
     <row r="789">
@@ -65027,10 +65007,10 @@
         <v>139</v>
       </c>
       <c r="B826" s="28" t="s">
+        <v>6765</v>
+      </c>
+      <c r="C826" s="28" t="s">
         <v>6766</v>
-      </c>
-      <c r="C826" s="28" t="s">
-        <v>6767</v>
       </c>
       <c r="D826" s="53" t="s">
         <v>3931</v>
@@ -66979,7 +66959,7 @@
         <v>4584</v>
       </c>
       <c r="D965" s="53" t="s">
-        <v>6768</v>
+        <v>6767</v>
       </c>
     </row>
     <row r="966">
@@ -68365,7 +68345,7 @@
         <v>5039</v>
       </c>
       <c r="D1064" s="53" t="s">
-        <v>6769</v>
+        <v>6768</v>
       </c>
     </row>
     <row r="1065">
@@ -68393,7 +68373,7 @@
         <v>5047</v>
       </c>
       <c r="D1066" s="53" t="s">
-        <v>6770</v>
+        <v>6769</v>
       </c>
     </row>
     <row r="1067">
@@ -68421,7 +68401,7 @@
         <v>5055</v>
       </c>
       <c r="D1068" s="53" t="s">
-        <v>6771</v>
+        <v>6770</v>
       </c>
     </row>
     <row r="1069">
@@ -68463,7 +68443,7 @@
         <v>5070</v>
       </c>
       <c r="D1071" s="54" t="s">
-        <v>6772</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="1072">
@@ -68533,7 +68513,7 @@
         <v>5086</v>
       </c>
       <c r="D1076" s="63" t="s">
-        <v>6773</v>
+        <v>6772</v>
       </c>
     </row>
     <row r="1077">
@@ -68575,7 +68555,7 @@
         <v>5100</v>
       </c>
       <c r="D1079" s="53" t="s">
-        <v>6774</v>
+        <v>6773</v>
       </c>
     </row>
     <row r="1080">
@@ -68701,7 +68681,7 @@
         <v>5141</v>
       </c>
       <c r="D1088" s="53" t="s">
-        <v>6775</v>
+        <v>6774</v>
       </c>
     </row>
     <row r="1089">
@@ -68757,7 +68737,7 @@
         <v>5159</v>
       </c>
       <c r="D1092" s="53" t="s">
-        <v>6776</v>
+        <v>6775</v>
       </c>
     </row>
     <row r="1093">
@@ -69104,7 +69084,7 @@
         <v>5286</v>
       </c>
       <c r="C1117" s="28" t="s">
-        <v>6777</v>
+        <v>6776</v>
       </c>
       <c r="D1117" s="61" t="s">
         <v>5289</v>
@@ -69639,7 +69619,7 @@
         <v>5477</v>
       </c>
       <c r="D1155" s="53" t="s">
-        <v>6778</v>
+        <v>6777</v>
       </c>
     </row>
     <row r="1156">
@@ -69846,7 +69826,7 @@
         <v>5541</v>
       </c>
       <c r="C1170" s="28" t="s">
-        <v>6779</v>
+        <v>6778</v>
       </c>
       <c r="D1170" s="54" t="s">
         <v>5544</v>
@@ -70882,10 +70862,10 @@
         <v>5885</v>
       </c>
       <c r="C1244" s="28" t="s">
+        <v>6779</v>
+      </c>
+      <c r="D1244" s="61" t="s">
         <v>6780</v>
-      </c>
-      <c r="D1244" s="61" t="s">
-        <v>6781</v>
       </c>
     </row>
     <row r="1245">
@@ -72209,13 +72189,13 @@
         <v>84</v>
       </c>
       <c r="B1339" s="28" t="s">
+        <v>6781</v>
+      </c>
+      <c r="C1339" s="27" t="s">
         <v>6782</v>
       </c>
-      <c r="C1339" s="27" t="s">
+      <c r="D1339" s="59" t="s">
         <v>6783</v>
-      </c>
-      <c r="D1339" s="59" t="s">
-        <v>6784</v>
       </c>
     </row>
     <row r="1340">
@@ -72394,7 +72374,7 @@
         <v>6387</v>
       </c>
       <c r="C1352" s="27" t="s">
-        <v>6785</v>
+        <v>6784</v>
       </c>
       <c r="D1352" s="81" t="s">
         <v>6390</v>
@@ -73007,13 +72987,13 @@
         <v>53</v>
       </c>
       <c r="B1396" s="28" t="s">
+        <v>6785</v>
+      </c>
+      <c r="C1396" s="27" t="s">
         <v>6786</v>
       </c>
-      <c r="C1396" s="27" t="s">
+      <c r="D1396" s="59" t="s">
         <v>6787</v>
-      </c>
-      <c r="D1396" s="59" t="s">
-        <v>6788</v>
       </c>
     </row>
     <row r="1397">

</xml_diff>

<commit_message>
Update letter cases (#170)
* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

---------

Co-authored-by: touge <touge1027@gmail.com>
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_DC9169F3_CEC1_48DA_9009_37A06AC1058B_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_2B9E84B6_F9B5_4F00_9170_DF49C5FE68A3_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_BCA54AE7_BFBC_438B_8516_CDCA8C8BDBB4_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DC20AA0D_D12E_40B9_B0F0_05AFBDC25C22_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2B9E84B6-F9B5-4F00-9170-DF49C5FE68A3}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC9169F3-CEC1-48DA-9009-37A06AC1058B}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{BCA54AE7-BFBC-438B-8516-CDCA8C8BDBB4}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC20AA0D-D12E-40B9-B0F0-05AFBDC25C22}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -20309,10 +20309,10 @@
     <t>已断开</t>
   </si>
   <si>
-    <t>no_dapp</t>
-  </si>
-  <si>
-    <t>No dapp</t>
+    <t>NO_DAPP</t>
+  </si>
+  <si>
+    <t>NO DAPP</t>
   </si>
   <si>
     <t>没有 Dapp</t>
@@ -53383,10 +53383,10 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC9169F3-CEC1-48DA-9009-37A06AC1058B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DC20AA0D-D12E-40B9-B0F0-05AFBDC25C22}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1480"/>
     </customSheetView>
-    <customSheetView guid="{2B9E84B6-F9B5-4F00-9170-DF49C5FE68A3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BCA54AE7-BFBC-438B-8516-CDCA8C8BDBB4}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1480"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Clarify the object that accessing public address is a dapp (#171)
* update client.xlsx

* update client.xlsx

* Update client.md and client XMLs

---------

Co-authored-by: touge <touge1027@gmail.com>
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_BCA54AE7_BFBC_438B_8516_CDCA8C8BDBB4_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DC20AA0D_D12E_40B9_B0F0_05AFBDC25C22_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_8D53E57C_7141_42D4_A230_52A8DF815194_.wvu.FilterData">'client strings'!$D$1:$D$1480</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B0932E88_E0A3_4451_8655_D2D6C56E7C32_.wvu.FilterData">'client strings'!$C$1:$C$1480</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{BCA54AE7-BFBC-438B-8516-CDCA8C8BDBB4}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC20AA0D-D12E-40B9-B0F0-05AFBDC25C22}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B0932E88-E0A3-4451-8655-D2D6C56E7C32}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8D53E57C-7141-42D4-A230-52A8DF815194}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -20195,10 +20195,10 @@
     <t>allow_dapp_access_public_address</t>
   </si>
   <si>
-    <t>Allow app to access your wallet balance and activity.</t>
-  </si>
-  <si>
-    <t>允许 App 访问你的钱包余额及活动。</t>
+    <t>Allow dapp to access your wallet balance and activity.</t>
+  </si>
+  <si>
+    <t>允许 Dapp 访问你的钱包余额及活动。</t>
   </si>
   <si>
     <t>request_permission</t>
@@ -53383,10 +53383,10 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DC20AA0D-D12E-40B9-B0F0-05AFBDC25C22}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8D53E57C-7141-42D4-A230-52A8DF815194}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1480"/>
     </customSheetView>
-    <customSheetView guid="{BCA54AE7-BFBC-438B-8516-CDCA8C8BDBB4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B0932E88-E0A3-4451-8655-D2D6C56E7C32}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1480"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update not supported deposit (#215)
* update client.xlsx

* Update client.md and client XMLs

* update client.xlsx

* Update client.md and client XMLs
</commit_message>
<xml_diff>
--- a/client.xlsx
+++ b/client.xlsx
@@ -7,13 +7,13 @@
     <sheet state="visible" name="ja" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_7C6CC3BC_601A_44AE_8568_08CCC77C36AD_.wvu.FilterData">'client strings'!$D$1:$D$1552</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_27E67D09_C4E7_40B9_BAF6_A13EE0BAF2AA_.wvu.FilterData">'client strings'!$C$1:$C$1552</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0CC4DADF_814D_45A4_BC08_7475624CF05D_.wvu.FilterData">'client strings'!$D$1:$D$1552</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_88B7786B_D1BC_4F5C_87B9_5B6CA8A5B605_.wvu.FilterData">'client strings'!$C$1:$C$1552</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{27E67D09-C4E7-40B9-BAF6-A13EE0BAF2AA}" name="过滤器1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7C6CC3BC-601A-44AE-8568-08CCC77C36AD}" name="过滤器2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88B7786B-D1BC-4F5C-87B9-5B6CA8A5B605}" name="过滤器1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0CC4DADF-814D-45A4-BC08-7475624CF05D}" name="过滤器2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -882,10 +882,10 @@
     <t>not_supported_deposit</t>
   </si>
   <si>
-    <t>Mixin Wallet does not support the deposit for %1$s. Please note that you can continue to transfer or withdraw the deposited %2$s. Read the document to **learn more**.</t>
-  </si>
-  <si>
-    <t>Mixin 钱包现已不支持 %1$s 充值，注意已转入的 %2$s 资产可以继续转账或提现，阅读文档**了解更多**。</t>
+    <t>Mixin ceases support for deposit service on the %1$s. You can continue to withdraw and transfer %1$s in the wallet balance. Read the document to **learn more**.</t>
+  </si>
+  <si>
+    <t>Mixin 已停止支持 %1$s 的充值服务。您可以继续提现和转账钱包余额中的 %1$s。**了解更多**请阅读文档。</t>
   </si>
   <si>
     <t>access_your_bots_list</t>
@@ -64979,10 +64979,10 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7C6CC3BC-601A-44AE-8568-08CCC77C36AD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0CC4DADF-814D-45A4-BC08-7475624CF05D}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$D$1552"/>
     </customSheetView>
-    <customSheetView guid="{27E67D09-C4E7-40B9-BAF6-A13EE0BAF2AA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{88B7786B-D1BC-4F5C-87B9-5B6CA8A5B605}" filter="1" showAutoFilter="1">
       <autoFilter ref="$C$1:$C$1552"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>